<commit_message>
Jan 31 2024 update
</commit_message>
<xml_diff>
--- a/SQL/leetcode - sql.xlsx
+++ b/SQL/leetcode - sql.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zw/Documents/Github/LeetCode_Practice/SQL/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E89EB693-F1E0-4C43-BF23-261835E52586}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABE4C4F2-BA6E-7542-A94A-EBF6EF615D78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2099,7 +2099,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="112" zoomScaleNormal="120" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F40" sqref="F40"/>
+      <selection pane="bottomLeft" activeCell="B40" sqref="B40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="28" defaultRowHeight="14" x14ac:dyDescent="0.15"/>

</xml_diff>

<commit_message>
Feb 1 2024 update
</commit_message>
<xml_diff>
--- a/SQL/leetcode - sql.xlsx
+++ b/SQL/leetcode - sql.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zw/Documents/Github/LeetCode_Practice/SQL/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABE4C4F2-BA6E-7542-A94A-EBF6EF615D78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A36A445A-876E-1445-9534-D3C684C6306C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="935" uniqueCount="462">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="945" uniqueCount="462">
   <si>
     <t>Title</t>
   </si>
@@ -696,9 +696,6 @@
   </si>
   <si>
     <t>这道题容易错，因为如果没有对应的值，那么我们期待返回null而非空集，一般这种事要用max或者min来选的</t>
-  </si>
-  <si>
-    <t>学会mod或者%如何应用</t>
   </si>
   <si>
     <t>学会使用update</t>
@@ -1258,9 +1255,6 @@
     <t>Case When &amp; Union ALL &amp; Not In &amp; Join</t>
   </si>
   <si>
-    <t>这道题考查四个点：1. 如何算平方(pow) 2. 如何算平方根(sqrt) 3. 如何找最小值(min) 4.如何保留两位小数(round)</t>
-  </si>
-  <si>
     <t>Case When &amp; Cal</t>
   </si>
   <si>
@@ -1268,9 +1262,6 @@
   </si>
   <si>
     <t>Case When &amp; Join &amp; Date &amp; Cal</t>
-  </si>
-  <si>
-    <t>的确比其他题目是有点复杂，不过我觉得这种题目到现在难度也只可能是medium而不能是hard，所以会还是要会的，对于这种题目，其实用cte会比较清晰</t>
   </si>
   <si>
     <t>我就算刷完了所有的leetcode，仍旧觉得pivot table算难题……
@@ -1594,6 +1585,21 @@
       </rPr>
       <t>：可以直接用老方法join，但是要注意了，这里join我们选择a表，但是a表是需要把所有满足条件的行都给挑出来的。所以我们直接可以两个join先把三个表给弄起来，然后在on中把三张表的关系一一列出来。</t>
     </r>
+  </si>
+  <si>
+    <t>这道题考查四个点：
+1. 如何算平方pow(a,b) -&gt; 对a取n次方
+2. 如何算平方根(sqrt) 
+3. 如何找最小值(min) 
+4.如何保留两位小数(round)</t>
+  </si>
+  <si>
+    <t>mysql是不能用date_trunc()的……神奇。那么我们就用date_format(day, '%Y-%m-%d')这种形式来规范日期</t>
+  </si>
+  <si>
+    <t>求余数：
+1. mod(a,b) -&gt; a/b的余数
+2. a%b -&gt; a/b的余数</t>
   </si>
 </sst>
 </file>
@@ -2097,9 +2103,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1C70A3A-EB9B-3540-8C26-B9C443B2B647}">
   <dimension ref="A1:I185"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="112" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B40" sqref="B40"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="112" zoomScaleNormal="120" workbookViewId="0">
+      <pane ySplit="6" topLeftCell="A49" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G50" sqref="G50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="28" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -2163,10 +2169,10 @@
         <v>1</v>
       </c>
       <c r="G6" s="45" t="s">
-        <v>452</v>
+        <v>449</v>
       </c>
       <c r="H6" s="12" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="I6" s="11" t="s">
         <v>194</v>
@@ -2213,7 +2219,7 @@
         <v>6</v>
       </c>
       <c r="I8" s="4" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="9" spans="1:9" s="27" customFormat="1" ht="76" thickBot="1" x14ac:dyDescent="0.2">
@@ -2236,7 +2242,7 @@
         <v>6</v>
       </c>
       <c r="I9" s="25" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="91" thickBot="1" x14ac:dyDescent="0.2">
@@ -2257,7 +2263,7 @@
         <v>6</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>453</v>
+        <v>450</v>
       </c>
     </row>
     <row r="11" spans="1:9" s="14" customFormat="1" ht="61" thickBot="1" x14ac:dyDescent="0.2">
@@ -2280,7 +2286,7 @@
         <v>6</v>
       </c>
       <c r="I11" s="4" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.2">
@@ -2330,7 +2336,7 @@
         <v>21</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C14" s="2"/>
       <c r="D14" s="19" t="s">
@@ -2343,7 +2349,7 @@
         <v>6</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>454</v>
+        <v>451</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="31" thickBot="1" x14ac:dyDescent="0.2">
@@ -2364,7 +2370,7 @@
         <v>6</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="31" thickBot="1" x14ac:dyDescent="0.2">
@@ -2410,7 +2416,7 @@
         <v>6</v>
       </c>
       <c r="I17" s="25" t="s">
-        <v>455</v>
+        <v>452</v>
       </c>
     </row>
     <row r="18" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.2">
@@ -2441,7 +2447,7 @@
         <v>29</v>
       </c>
       <c r="B19" s="16" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="C19" s="16"/>
       <c r="D19" s="21"/>
@@ -2456,7 +2462,7 @@
         <v>6</v>
       </c>
       <c r="I19" s="29" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="20" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.2">
@@ -2485,7 +2491,7 @@
         <v>31</v>
       </c>
       <c r="B21" s="41" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="C21" s="2"/>
       <c r="D21" s="19" t="s">
@@ -2498,7 +2504,7 @@
         <v>6</v>
       </c>
       <c r="I21" s="40" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="22" spans="1:9" s="27" customFormat="1" ht="46" thickBot="1" x14ac:dyDescent="0.2">
@@ -2506,7 +2512,7 @@
         <v>32</v>
       </c>
       <c r="B22" s="50" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="C22" s="25"/>
       <c r="D22" s="26"/>
@@ -2521,7 +2527,7 @@
         <v>6</v>
       </c>
       <c r="I22" s="51" t="s">
-        <v>456</v>
+        <v>453</v>
       </c>
     </row>
     <row r="23" spans="1:9" ht="31" thickBot="1" x14ac:dyDescent="0.2">
@@ -2542,7 +2548,7 @@
         <v>6</v>
       </c>
       <c r="I23" s="40" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
     <row r="24" spans="1:9" s="17" customFormat="1" ht="91" thickBot="1" x14ac:dyDescent="0.2">
@@ -2567,7 +2573,7 @@
         <v>6</v>
       </c>
       <c r="I24" s="29" t="s">
-        <v>457</v>
+        <v>454</v>
       </c>
     </row>
     <row r="25" spans="1:9" s="14" customFormat="1" ht="46" thickBot="1" x14ac:dyDescent="0.2">
@@ -2590,7 +2596,7 @@
         <v>6</v>
       </c>
       <c r="I25" s="53" t="s">
-        <v>458</v>
+        <v>455</v>
       </c>
     </row>
     <row r="26" spans="1:9" s="17" customFormat="1" ht="409.6" thickBot="1" x14ac:dyDescent="0.2">
@@ -2598,7 +2604,7 @@
         <v>35</v>
       </c>
       <c r="B26" s="16" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="C26" s="28" t="s">
         <v>34</v>
@@ -2615,7 +2621,7 @@
         <v>6</v>
       </c>
       <c r="I26" s="29" t="s">
-        <v>459</v>
+        <v>456</v>
       </c>
     </row>
     <row r="27" spans="1:9" ht="31" thickBot="1" x14ac:dyDescent="0.2">
@@ -2623,7 +2629,7 @@
         <v>37</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="C27" s="2"/>
       <c r="E27" s="19" t="s">
@@ -2636,7 +2642,7 @@
         <v>6</v>
       </c>
       <c r="I27" s="24" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="28" spans="1:9" ht="46" thickBot="1" x14ac:dyDescent="0.2">
@@ -2644,7 +2650,7 @@
         <v>8</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="C28" s="1"/>
       <c r="D28" s="19" t="s">
@@ -2657,7 +2663,7 @@
         <v>6</v>
       </c>
       <c r="I28" s="32" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="29" spans="1:9" ht="210" x14ac:dyDescent="0.15">
@@ -2677,7 +2683,7 @@
         <v>6</v>
       </c>
       <c r="I29" s="32" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="30" spans="1:9" s="17" customFormat="1" ht="255" x14ac:dyDescent="0.15">
@@ -2685,7 +2691,7 @@
         <v>40</v>
       </c>
       <c r="B30" s="17" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="D30" s="21"/>
       <c r="E30" s="21"/>
@@ -2739,7 +2745,7 @@
         <v>6</v>
       </c>
       <c r="I32" s="32" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="33" spans="1:9" ht="46" thickBot="1" x14ac:dyDescent="0.2">
@@ -2759,7 +2765,7 @@
         <v>6</v>
       </c>
       <c r="I33" s="32" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
     </row>
     <row r="34" spans="1:9" ht="15" x14ac:dyDescent="0.15">
@@ -2841,7 +2847,7 @@
         <v>6</v>
       </c>
       <c r="I37" s="35" t="s">
-        <v>460</v>
+        <v>457</v>
       </c>
     </row>
     <row r="38" spans="1:9" s="17" customFormat="1" ht="180" x14ac:dyDescent="0.15">
@@ -2866,7 +2872,7 @@
         <v>6</v>
       </c>
       <c r="I38" s="33" t="s">
-        <v>461</v>
+        <v>458</v>
       </c>
     </row>
     <row r="39" spans="1:9" ht="30" x14ac:dyDescent="0.15">
@@ -2874,7 +2880,7 @@
         <v>50</v>
       </c>
       <c r="B39" s="6" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="E39" s="19" t="s">
         <v>6</v>
@@ -2909,7 +2915,7 @@
         <v>6</v>
       </c>
       <c r="I40" s="32" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
     </row>
     <row r="41" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.2">
@@ -2917,7 +2923,7 @@
         <v>51</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="D41" s="19" t="s">
         <v>6</v>
@@ -2929,7 +2935,7 @@
         <v>6</v>
       </c>
       <c r="I41" s="32" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
     </row>
     <row r="42" spans="1:9" ht="30" x14ac:dyDescent="0.15">
@@ -2937,16 +2943,19 @@
         <v>52</v>
       </c>
       <c r="B42" s="6" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="E42" s="19" t="s">
         <v>6</v>
       </c>
+      <c r="G42" s="44" t="s">
+        <v>6</v>
+      </c>
       <c r="H42" s="19" t="s">
         <v>6</v>
       </c>
       <c r="I42" s="32" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="43" spans="1:9" ht="30" x14ac:dyDescent="0.15">
@@ -2954,9 +2963,12 @@
         <v>53</v>
       </c>
       <c r="B43" s="6" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="D43" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="G43" s="44" t="s">
         <v>6</v>
       </c>
       <c r="H43" s="19" t="s">
@@ -2966,12 +2978,12 @@
         <v>213</v>
       </c>
     </row>
-    <row r="44" spans="1:9" s="27" customFormat="1" ht="30" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:9" s="27" customFormat="1" ht="75" x14ac:dyDescent="0.15">
       <c r="A44" s="27" t="s">
         <v>160</v>
       </c>
       <c r="B44" s="27" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="C44" s="27" t="s">
         <v>161</v>
@@ -2981,12 +2993,14 @@
         <v>6</v>
       </c>
       <c r="F44" s="26"/>
-      <c r="G44" s="47"/>
+      <c r="G44" s="47" t="s">
+        <v>6</v>
+      </c>
       <c r="H44" s="26" t="s">
         <v>6</v>
       </c>
       <c r="I44" s="35" t="s">
-        <v>389</v>
+        <v>459</v>
       </c>
     </row>
     <row r="45" spans="1:9" ht="15" x14ac:dyDescent="0.15">
@@ -3002,6 +3016,9 @@
       <c r="D45" s="19" t="s">
         <v>6</v>
       </c>
+      <c r="G45" s="44" t="s">
+        <v>6</v>
+      </c>
       <c r="H45" s="19" t="s">
         <v>6</v>
       </c>
@@ -3019,6 +3036,9 @@
       <c r="E46" s="19" t="s">
         <v>6</v>
       </c>
+      <c r="G46" s="44" t="s">
+        <v>6</v>
+      </c>
       <c r="H46" s="19" t="s">
         <v>6</v>
       </c>
@@ -3026,12 +3046,12 @@
         <v>216</v>
       </c>
     </row>
-    <row r="47" spans="1:9" ht="45" x14ac:dyDescent="0.15">
+    <row r="47" spans="1:9" ht="30" x14ac:dyDescent="0.15">
       <c r="A47" s="6" t="s">
         <v>132</v>
       </c>
       <c r="B47" s="6" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="C47" s="6" t="s">
         <v>73</v>
@@ -3039,11 +3059,14 @@
       <c r="F47" s="19" t="s">
         <v>6</v>
       </c>
+      <c r="G47" s="44" t="s">
+        <v>6</v>
+      </c>
       <c r="H47" s="19" t="s">
         <v>6</v>
       </c>
       <c r="I47" s="32" t="s">
-        <v>393</v>
+        <v>460</v>
       </c>
     </row>
     <row r="48" spans="1:9" s="17" customFormat="1" ht="75" x14ac:dyDescent="0.15">
@@ -3058,12 +3081,14 @@
       <c r="F48" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="G48" s="48"/>
+      <c r="G48" s="48" t="s">
+        <v>6</v>
+      </c>
       <c r="H48" s="21" t="s">
         <v>6</v>
       </c>
       <c r="I48" s="33" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
     </row>
     <row r="49" spans="1:9" s="14" customFormat="1" ht="30" x14ac:dyDescent="0.15">
@@ -3071,14 +3096,16 @@
         <v>166</v>
       </c>
       <c r="B49" s="14" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="D49" s="20" t="s">
         <v>6</v>
       </c>
       <c r="E49" s="20"/>
       <c r="F49" s="20"/>
-      <c r="G49" s="46"/>
+      <c r="G49" s="46" t="s">
+        <v>6</v>
+      </c>
       <c r="H49" s="20" t="s">
         <v>6</v>
       </c>
@@ -3086,7 +3113,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="50" spans="1:9" ht="15" x14ac:dyDescent="0.15">
+    <row r="50" spans="1:9" ht="45" x14ac:dyDescent="0.15">
       <c r="A50" s="6" t="s">
         <v>54</v>
       </c>
@@ -3096,11 +3123,14 @@
       <c r="D50" s="19" t="s">
         <v>6</v>
       </c>
+      <c r="G50" s="44" t="s">
+        <v>6</v>
+      </c>
       <c r="H50" s="19" t="s">
         <v>6</v>
       </c>
       <c r="I50" s="32" t="s">
-        <v>219</v>
+        <v>461</v>
       </c>
     </row>
     <row r="51" spans="1:9" s="17" customFormat="1" ht="60" x14ac:dyDescent="0.15">
@@ -3115,12 +3145,14 @@
         <v>6</v>
       </c>
       <c r="F51" s="21"/>
-      <c r="G51" s="48"/>
+      <c r="G51" s="48" t="s">
+        <v>6</v>
+      </c>
       <c r="H51" s="21" t="s">
         <v>6</v>
       </c>
       <c r="I51" s="33" t="s">
-        <v>395</v>
+        <v>392</v>
       </c>
     </row>
     <row r="52" spans="1:9" s="27" customFormat="1" ht="15" x14ac:dyDescent="0.15">
@@ -3128,7 +3160,7 @@
         <v>55</v>
       </c>
       <c r="B52" s="27" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
       <c r="D52" s="26" t="s">
         <v>6</v>
@@ -3140,7 +3172,7 @@
         <v>6</v>
       </c>
       <c r="I52" s="35" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="53" spans="1:9" ht="45" x14ac:dyDescent="0.15">
@@ -3148,16 +3180,16 @@
         <v>57</v>
       </c>
       <c r="B53" s="6" t="s">
+        <v>220</v>
+      </c>
+      <c r="E53" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="H53" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="I53" s="32" t="s">
         <v>221</v>
-      </c>
-      <c r="E53" s="19" t="s">
-        <v>6</v>
-      </c>
-      <c r="H53" s="19" t="s">
-        <v>6</v>
-      </c>
-      <c r="I53" s="32" t="s">
-        <v>222</v>
       </c>
     </row>
     <row r="54" spans="1:9" ht="15" x14ac:dyDescent="0.15">
@@ -3174,7 +3206,7 @@
         <v>6</v>
       </c>
       <c r="I54" s="32" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="55" spans="1:9" ht="15" x14ac:dyDescent="0.15">
@@ -3191,7 +3223,7 @@
         <v>6</v>
       </c>
       <c r="I55" s="32" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="56" spans="1:9" ht="15" x14ac:dyDescent="0.15">
@@ -3208,7 +3240,7 @@
         <v>6</v>
       </c>
       <c r="I56" s="32" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="57" spans="1:9" ht="45" x14ac:dyDescent="0.15">
@@ -3216,7 +3248,7 @@
         <v>61</v>
       </c>
       <c r="B57" s="6" t="s">
-        <v>397</v>
+        <v>394</v>
       </c>
       <c r="E57" s="19" t="s">
         <v>6</v>
@@ -3225,7 +3257,7 @@
         <v>6</v>
       </c>
       <c r="I57" s="32" t="s">
-        <v>398</v>
+        <v>395</v>
       </c>
     </row>
     <row r="58" spans="1:9" ht="15" x14ac:dyDescent="0.15">
@@ -3242,7 +3274,7 @@
         <v>6</v>
       </c>
       <c r="I58" s="32" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="59" spans="1:9" ht="30" x14ac:dyDescent="0.15">
@@ -3262,7 +3294,7 @@
         <v>6</v>
       </c>
       <c r="I59" s="32" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="60" spans="1:9" ht="45" x14ac:dyDescent="0.15">
@@ -3279,7 +3311,7 @@
         <v>6</v>
       </c>
       <c r="I60" s="32" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
     </row>
     <row r="61" spans="1:9" ht="15" x14ac:dyDescent="0.15">
@@ -3299,7 +3331,7 @@
         <v>6</v>
       </c>
       <c r="I61" s="32" t="s">
-        <v>400</v>
+        <v>397</v>
       </c>
     </row>
     <row r="62" spans="1:9" s="14" customFormat="1" ht="45" x14ac:dyDescent="0.15">
@@ -3307,7 +3339,7 @@
         <v>66</v>
       </c>
       <c r="B62" s="14" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="D62" s="20" t="s">
         <v>6</v>
@@ -3319,7 +3351,7 @@
         <v>6</v>
       </c>
       <c r="I62" s="34" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="63" spans="1:9" ht="46" thickBot="1" x14ac:dyDescent="0.2">
@@ -3327,7 +3359,7 @@
         <v>67</v>
       </c>
       <c r="B63" s="6" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D63" s="19" t="s">
         <v>6</v>
@@ -3336,7 +3368,7 @@
         <v>6</v>
       </c>
       <c r="I63" s="32" t="s">
-        <v>401</v>
+        <v>398</v>
       </c>
     </row>
     <row r="64" spans="1:9" ht="31" thickBot="1" x14ac:dyDescent="0.2">
@@ -3344,7 +3376,7 @@
         <v>68</v>
       </c>
       <c r="B64" s="41" t="s">
-        <v>402</v>
+        <v>399</v>
       </c>
       <c r="C64" s="2"/>
       <c r="F64" s="19" t="s">
@@ -3354,7 +3386,7 @@
         <v>6</v>
       </c>
       <c r="I64" s="40" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="65" spans="1:9" s="14" customFormat="1" ht="105" x14ac:dyDescent="0.15">
@@ -3362,7 +3394,7 @@
         <v>69</v>
       </c>
       <c r="B65" s="14" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="D65" s="20"/>
       <c r="E65" s="20" t="s">
@@ -3374,7 +3406,7 @@
         <v>6</v>
       </c>
       <c r="I65" s="34" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
     </row>
     <row r="66" spans="1:9" ht="15" x14ac:dyDescent="0.15">
@@ -3382,7 +3414,7 @@
         <v>70</v>
       </c>
       <c r="B66" s="6" t="s">
-        <v>404</v>
+        <v>401</v>
       </c>
       <c r="E66" s="19" t="s">
         <v>6</v>
@@ -3391,7 +3423,7 @@
         <v>6</v>
       </c>
       <c r="I66" s="32" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="67" spans="1:9" ht="15" x14ac:dyDescent="0.15">
@@ -3408,7 +3440,7 @@
         <v>6</v>
       </c>
       <c r="I67" s="32" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="68" spans="1:9" ht="15" x14ac:dyDescent="0.15">
@@ -3425,7 +3457,7 @@
         <v>6</v>
       </c>
       <c r="I68" s="32" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="69" spans="1:9" ht="30" x14ac:dyDescent="0.15">
@@ -3445,7 +3477,7 @@
         <v>6</v>
       </c>
       <c r="I69" s="32" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="70" spans="1:9" s="17" customFormat="1" ht="90" x14ac:dyDescent="0.15">
@@ -3453,7 +3485,7 @@
         <v>75</v>
       </c>
       <c r="B70" s="17" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="D70" s="21"/>
       <c r="E70" s="21"/>
@@ -3465,7 +3497,7 @@
         <v>6</v>
       </c>
       <c r="I70" s="33" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.15">
@@ -3482,7 +3514,7 @@
         <v>6</v>
       </c>
       <c r="I71" s="6" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="72" spans="1:9" ht="30" x14ac:dyDescent="0.15">
@@ -3499,7 +3531,7 @@
         <v>6</v>
       </c>
       <c r="I72" s="32" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="73" spans="1:9" ht="30" x14ac:dyDescent="0.15">
@@ -3516,7 +3548,7 @@
         <v>6</v>
       </c>
       <c r="I73" s="32" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="74" spans="1:9" ht="15" x14ac:dyDescent="0.15">
@@ -3533,7 +3565,7 @@
         <v>6</v>
       </c>
       <c r="I74" s="32" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="75" spans="1:9" s="14" customFormat="1" ht="75" x14ac:dyDescent="0.15">
@@ -3553,7 +3585,7 @@
         <v>6</v>
       </c>
       <c r="I75" s="34" t="s">
-        <v>405</v>
+        <v>402</v>
       </c>
     </row>
     <row r="76" spans="1:9" ht="60" x14ac:dyDescent="0.15">
@@ -3570,7 +3602,7 @@
         <v>6</v>
       </c>
       <c r="I76" s="32" t="s">
-        <v>406</v>
+        <v>403</v>
       </c>
     </row>
     <row r="77" spans="1:9" ht="30" x14ac:dyDescent="0.15">
@@ -3578,7 +3610,7 @@
         <v>85</v>
       </c>
       <c r="B77" s="6" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="F77" s="19" t="s">
         <v>6</v>
@@ -3587,7 +3619,7 @@
         <v>6</v>
       </c>
       <c r="I77" s="32" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="78" spans="1:9" ht="30" x14ac:dyDescent="0.15">
@@ -3595,7 +3627,7 @@
         <v>86</v>
       </c>
       <c r="B78" s="6" t="s">
-        <v>407</v>
+        <v>404</v>
       </c>
       <c r="E78" s="19" t="s">
         <v>6</v>
@@ -3604,7 +3636,7 @@
         <v>6</v>
       </c>
       <c r="I78" s="32" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="79" spans="1:9" ht="15" x14ac:dyDescent="0.15">
@@ -3612,7 +3644,7 @@
         <v>87</v>
       </c>
       <c r="B79" s="6" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="D79" s="19" t="s">
         <v>6</v>
@@ -3621,7 +3653,7 @@
         <v>6</v>
       </c>
       <c r="I79" s="32" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="80" spans="1:9" ht="45" x14ac:dyDescent="0.15">
@@ -3629,7 +3661,7 @@
         <v>88</v>
       </c>
       <c r="B80" s="6" t="s">
-        <v>409</v>
+        <v>406</v>
       </c>
       <c r="E80" s="19" t="s">
         <v>6</v>
@@ -3638,7 +3670,7 @@
         <v>6</v>
       </c>
       <c r="I80" s="32" t="s">
-        <v>411</v>
+        <v>408</v>
       </c>
     </row>
     <row r="81" spans="1:9" ht="30" x14ac:dyDescent="0.15">
@@ -3646,7 +3678,7 @@
         <v>89</v>
       </c>
       <c r="B81" s="6" t="s">
-        <v>413</v>
+        <v>410</v>
       </c>
       <c r="D81" s="19" t="s">
         <v>6</v>
@@ -3655,7 +3687,7 @@
         <v>6</v>
       </c>
       <c r="I81" s="32" t="s">
-        <v>412</v>
+        <v>409</v>
       </c>
     </row>
     <row r="82" spans="1:9" ht="15" x14ac:dyDescent="0.15">
@@ -3663,7 +3695,7 @@
         <v>90</v>
       </c>
       <c r="B82" s="6" t="s">
-        <v>410</v>
+        <v>407</v>
       </c>
       <c r="E82" s="19" t="s">
         <v>6</v>
@@ -3672,7 +3704,7 @@
         <v>6</v>
       </c>
       <c r="I82" s="32" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="83" spans="1:9" ht="45" x14ac:dyDescent="0.15">
@@ -3680,7 +3712,7 @@
         <v>91</v>
       </c>
       <c r="B83" s="6" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="F83" s="19" t="s">
         <v>6</v>
@@ -3689,7 +3721,7 @@
         <v>6</v>
       </c>
       <c r="I83" s="32" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="84" spans="1:9" ht="15" x14ac:dyDescent="0.15">
@@ -3697,7 +3729,7 @@
         <v>92</v>
       </c>
       <c r="B84" s="6" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="E84" s="19" t="s">
         <v>6</v>
@@ -3706,7 +3738,7 @@
         <v>6</v>
       </c>
       <c r="I84" s="32" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="85" spans="1:9" s="17" customFormat="1" ht="45" x14ac:dyDescent="0.15">
@@ -3714,7 +3746,7 @@
         <v>93</v>
       </c>
       <c r="B85" s="17" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
       <c r="D85" s="21"/>
       <c r="E85" s="21" t="s">
@@ -3726,7 +3758,7 @@
         <v>6</v>
       </c>
       <c r="I85" s="33" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="86" spans="1:9" ht="15" x14ac:dyDescent="0.15">
@@ -3734,7 +3766,7 @@
         <v>94</v>
       </c>
       <c r="B86" s="6" t="s">
-        <v>416</v>
+        <v>413</v>
       </c>
       <c r="D86" s="19" t="s">
         <v>6</v>
@@ -3743,7 +3775,7 @@
         <v>6</v>
       </c>
       <c r="I86" s="32" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="87" spans="1:9" ht="15" x14ac:dyDescent="0.15">
@@ -3751,7 +3783,7 @@
         <v>95</v>
       </c>
       <c r="B87" s="6" t="s">
-        <v>417</v>
+        <v>414</v>
       </c>
       <c r="E87" s="19" t="s">
         <v>6</v>
@@ -3760,7 +3792,7 @@
         <v>6</v>
       </c>
       <c r="I87" s="32" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="88" spans="1:9" s="17" customFormat="1" ht="150" x14ac:dyDescent="0.15">
@@ -3768,7 +3800,7 @@
         <v>98</v>
       </c>
       <c r="B88" s="17" t="s">
-        <v>418</v>
+        <v>415</v>
       </c>
       <c r="C88" s="33"/>
       <c r="D88" s="21"/>
@@ -3781,7 +3813,7 @@
         <v>6</v>
       </c>
       <c r="I88" s="33" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
     </row>
     <row r="89" spans="1:9" ht="15" x14ac:dyDescent="0.15">
@@ -3798,7 +3830,7 @@
         <v>6</v>
       </c>
       <c r="I89" s="32" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="90" spans="1:9" ht="15" x14ac:dyDescent="0.15">
@@ -3815,7 +3847,7 @@
         <v>6</v>
       </c>
       <c r="I90" s="32" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="91" spans="1:9" ht="15" x14ac:dyDescent="0.15">
@@ -3823,7 +3855,7 @@
         <v>99</v>
       </c>
       <c r="B91" s="6" t="s">
-        <v>420</v>
+        <v>417</v>
       </c>
       <c r="E91" s="19" t="s">
         <v>6</v>
@@ -3832,7 +3864,7 @@
         <v>6</v>
       </c>
       <c r="I91" s="32" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="92" spans="1:9" ht="15" x14ac:dyDescent="0.15">
@@ -3840,7 +3872,7 @@
         <v>100</v>
       </c>
       <c r="B92" s="6" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="E92" s="19" t="s">
         <v>6</v>
@@ -3849,7 +3881,7 @@
         <v>6</v>
       </c>
       <c r="I92" s="32" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="93" spans="1:9" s="14" customFormat="1" ht="75" x14ac:dyDescent="0.15">
@@ -3869,7 +3901,7 @@
         <v>6</v>
       </c>
       <c r="I93" s="34" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="94" spans="1:9" ht="15" x14ac:dyDescent="0.15">
@@ -3889,7 +3921,7 @@
         <v>6</v>
       </c>
       <c r="I94" s="32" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="95" spans="1:9" ht="30" x14ac:dyDescent="0.15">
@@ -3897,7 +3929,7 @@
         <v>103</v>
       </c>
       <c r="B95" s="6" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="D95" s="19" t="s">
         <v>6</v>
@@ -3906,7 +3938,7 @@
         <v>6</v>
       </c>
       <c r="I95" s="32" t="s">
-        <v>421</v>
+        <v>418</v>
       </c>
     </row>
     <row r="96" spans="1:9" s="27" customFormat="1" ht="60" x14ac:dyDescent="0.15">
@@ -3914,7 +3946,7 @@
         <v>104</v>
       </c>
       <c r="B96" s="27" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="D96" s="26" t="s">
         <v>6</v>
@@ -3926,7 +3958,7 @@
         <v>6</v>
       </c>
       <c r="I96" s="35" t="s">
-        <v>422</v>
+        <v>419</v>
       </c>
     </row>
     <row r="97" spans="1:9" ht="15" x14ac:dyDescent="0.15">
@@ -3934,7 +3966,7 @@
         <v>105</v>
       </c>
       <c r="B97" s="6" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="E97" s="19" t="s">
         <v>6</v>
@@ -3943,7 +3975,7 @@
         <v>6</v>
       </c>
       <c r="I97" s="32" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="98" spans="1:9" s="27" customFormat="1" ht="45" x14ac:dyDescent="0.15">
@@ -3951,7 +3983,7 @@
         <v>106</v>
       </c>
       <c r="B98" s="27" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
       <c r="D98" s="26"/>
       <c r="E98" s="26" t="s">
@@ -3963,7 +3995,7 @@
         <v>6</v>
       </c>
       <c r="I98" s="35" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="99" spans="1:9" ht="45" x14ac:dyDescent="0.15">
@@ -3971,7 +4003,7 @@
         <v>107</v>
       </c>
       <c r="B99" s="6" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="D99" s="19" t="s">
         <v>6</v>
@@ -3980,7 +4012,7 @@
         <v>6</v>
       </c>
       <c r="I99" s="32" t="s">
-        <v>424</v>
+        <v>421</v>
       </c>
     </row>
     <row r="100" spans="1:9" ht="15" x14ac:dyDescent="0.15">
@@ -3997,7 +4029,7 @@
         <v>6</v>
       </c>
       <c r="I100" s="32" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="101" spans="1:9" s="17" customFormat="1" ht="180" x14ac:dyDescent="0.15">
@@ -4005,7 +4037,7 @@
         <v>112</v>
       </c>
       <c r="B101" s="17" t="s">
-        <v>425</v>
+        <v>422</v>
       </c>
       <c r="D101" s="21"/>
       <c r="E101" s="21"/>
@@ -4017,7 +4049,7 @@
         <v>6</v>
       </c>
       <c r="I101" s="33" t="s">
-        <v>426</v>
+        <v>423</v>
       </c>
     </row>
     <row r="102" spans="1:9" ht="15" x14ac:dyDescent="0.15">
@@ -4034,7 +4066,7 @@
         <v>6</v>
       </c>
       <c r="I102" s="32" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="103" spans="1:9" ht="15" x14ac:dyDescent="0.15">
@@ -4042,7 +4074,7 @@
         <v>110</v>
       </c>
       <c r="B103" s="6" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="D103" s="19" t="s">
         <v>6</v>
@@ -4051,7 +4083,7 @@
         <v>6</v>
       </c>
       <c r="I103" s="32" t="s">
-        <v>427</v>
+        <v>424</v>
       </c>
     </row>
     <row r="104" spans="1:9" ht="60" x14ac:dyDescent="0.15">
@@ -4059,7 +4091,7 @@
         <v>113</v>
       </c>
       <c r="B104" s="6" t="s">
-        <v>428</v>
+        <v>425</v>
       </c>
       <c r="E104" s="19" t="s">
         <v>6</v>
@@ -4068,7 +4100,7 @@
         <v>6</v>
       </c>
       <c r="I104" s="32" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="105" spans="1:9" ht="45" x14ac:dyDescent="0.15">
@@ -4076,7 +4108,7 @@
         <v>115</v>
       </c>
       <c r="B105" s="6" t="s">
-        <v>429</v>
+        <v>426</v>
       </c>
       <c r="E105" s="19" t="s">
         <v>6</v>
@@ -4085,7 +4117,7 @@
         <v>6</v>
       </c>
       <c r="I105" s="32" t="s">
-        <v>430</v>
+        <v>427</v>
       </c>
     </row>
     <row r="106" spans="1:9" s="27" customFormat="1" ht="90" x14ac:dyDescent="0.15">
@@ -4093,7 +4125,7 @@
         <v>118</v>
       </c>
       <c r="B106" s="27" t="s">
-        <v>431</v>
+        <v>428</v>
       </c>
       <c r="D106" s="26"/>
       <c r="E106" s="26"/>
@@ -4105,7 +4137,7 @@
         <v>6</v>
       </c>
       <c r="I106" s="35" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="107" spans="1:9" ht="15" x14ac:dyDescent="0.15">
@@ -4122,7 +4154,7 @@
         <v>6</v>
       </c>
       <c r="I107" s="32" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="108" spans="1:9" s="17" customFormat="1" ht="45" x14ac:dyDescent="0.15">
@@ -4130,7 +4162,7 @@
         <v>119</v>
       </c>
       <c r="B108" s="17" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="D108" s="21"/>
       <c r="E108" s="21"/>
@@ -4142,7 +4174,7 @@
         <v>6</v>
       </c>
       <c r="I108" s="33" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="109" spans="1:9" ht="15" x14ac:dyDescent="0.15">
@@ -4150,7 +4182,7 @@
         <v>120</v>
       </c>
       <c r="B109" s="6" t="s">
-        <v>416</v>
+        <v>413</v>
       </c>
       <c r="E109" s="19" t="s">
         <v>6</v>
@@ -4159,7 +4191,7 @@
         <v>6</v>
       </c>
       <c r="I109" s="32" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="110" spans="1:9" ht="60" x14ac:dyDescent="0.15">
@@ -4176,7 +4208,7 @@
         <v>6</v>
       </c>
       <c r="I110" s="32" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="111" spans="1:9" ht="15" x14ac:dyDescent="0.15">
@@ -4193,7 +4225,7 @@
         <v>6</v>
       </c>
       <c r="I111" s="32" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="112" spans="1:9" s="14" customFormat="1" ht="46" x14ac:dyDescent="0.2">
@@ -4201,7 +4233,7 @@
         <v>124</v>
       </c>
       <c r="B112" s="42" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C112" s="14" t="s">
         <v>121</v>
@@ -4216,7 +4248,7 @@
         <v>6</v>
       </c>
       <c r="I112" s="34" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="113" spans="1:9" ht="15" x14ac:dyDescent="0.15">
@@ -4233,7 +4265,7 @@
         <v>6</v>
       </c>
       <c r="I113" s="32" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="114" spans="1:9" ht="30" x14ac:dyDescent="0.15">
@@ -4241,7 +4273,7 @@
         <v>125</v>
       </c>
       <c r="B114" s="6" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="D114" s="19" t="s">
         <v>6</v>
@@ -4250,7 +4282,7 @@
         <v>6</v>
       </c>
       <c r="I114" s="32" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="115" spans="1:9" s="17" customFormat="1" ht="30" x14ac:dyDescent="0.15">
@@ -4258,7 +4290,7 @@
         <v>126</v>
       </c>
       <c r="B115" s="17" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
       <c r="D115" s="21"/>
       <c r="E115" s="21" t="s">
@@ -4270,7 +4302,7 @@
         <v>6</v>
       </c>
       <c r="I115" s="33" t="s">
-        <v>434</v>
+        <v>431</v>
       </c>
     </row>
     <row r="116" spans="1:9" ht="15" x14ac:dyDescent="0.15">
@@ -4278,7 +4310,7 @@
         <v>127</v>
       </c>
       <c r="B116" s="6" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="E116" s="19" t="s">
         <v>6</v>
@@ -4287,7 +4319,7 @@
         <v>6</v>
       </c>
       <c r="I116" s="32" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="117" spans="1:9" s="27" customFormat="1" ht="30" x14ac:dyDescent="0.15">
@@ -4295,7 +4327,7 @@
         <v>128</v>
       </c>
       <c r="B117" s="27" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="D117" s="26"/>
       <c r="E117" s="26" t="s">
@@ -4307,7 +4339,7 @@
         <v>6</v>
       </c>
       <c r="I117" s="35" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="118" spans="1:9" ht="45" x14ac:dyDescent="0.15">
@@ -4324,7 +4356,7 @@
         <v>6</v>
       </c>
       <c r="I118" s="32" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="119" spans="1:9" ht="15" x14ac:dyDescent="0.15">
@@ -4332,7 +4364,7 @@
         <v>130</v>
       </c>
       <c r="B119" s="6" t="s">
-        <v>429</v>
+        <v>426</v>
       </c>
       <c r="E119" s="19" t="s">
         <v>6</v>
@@ -4341,7 +4373,7 @@
         <v>6</v>
       </c>
       <c r="I119" s="32" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="120" spans="1:9" s="17" customFormat="1" ht="15" x14ac:dyDescent="0.15">
@@ -4349,7 +4381,7 @@
         <v>136</v>
       </c>
       <c r="B120" s="17" t="s">
-        <v>437</v>
+        <v>434</v>
       </c>
       <c r="D120" s="21"/>
       <c r="E120" s="21"/>
@@ -4361,7 +4393,7 @@
         <v>6</v>
       </c>
       <c r="I120" s="33" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="121" spans="1:9" s="27" customFormat="1" ht="60" x14ac:dyDescent="0.15">
@@ -4369,7 +4401,7 @@
         <v>133</v>
       </c>
       <c r="B121" s="27" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="D121" s="26" t="s">
         <v>6</v>
@@ -4381,7 +4413,7 @@
         <v>6</v>
       </c>
       <c r="I121" s="35" t="s">
-        <v>438</v>
+        <v>435</v>
       </c>
     </row>
     <row r="122" spans="1:9" ht="15" x14ac:dyDescent="0.15">
@@ -4389,16 +4421,16 @@
         <v>135</v>
       </c>
       <c r="B122" s="6" t="s">
+        <v>276</v>
+      </c>
+      <c r="D122" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="H122" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="I122" s="32" t="s">
         <v>277</v>
-      </c>
-      <c r="D122" s="19" t="s">
-        <v>6</v>
-      </c>
-      <c r="H122" s="19" t="s">
-        <v>6</v>
-      </c>
-      <c r="I122" s="32" t="s">
-        <v>278</v>
       </c>
     </row>
     <row r="123" spans="1:9" ht="30" x14ac:dyDescent="0.15">
@@ -4406,7 +4438,7 @@
         <v>131</v>
       </c>
       <c r="B123" s="6" t="s">
-        <v>439</v>
+        <v>436</v>
       </c>
       <c r="E123" s="19" t="s">
         <v>6</v>
@@ -4415,7 +4447,7 @@
         <v>6</v>
       </c>
       <c r="I123" s="32" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="124" spans="1:9" ht="60" x14ac:dyDescent="0.15">
@@ -4423,16 +4455,16 @@
         <v>137</v>
       </c>
       <c r="B124" s="6" t="s">
+        <v>279</v>
+      </c>
+      <c r="D124" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="H124" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="I124" s="32" t="s">
         <v>280</v>
-      </c>
-      <c r="D124" s="19" t="s">
-        <v>6</v>
-      </c>
-      <c r="H124" s="19" t="s">
-        <v>6</v>
-      </c>
-      <c r="I124" s="32" t="s">
-        <v>281</v>
       </c>
     </row>
     <row r="125" spans="1:9" s="27" customFormat="1" ht="15" x14ac:dyDescent="0.15">
@@ -4440,7 +4472,7 @@
         <v>138</v>
       </c>
       <c r="B125" s="27" t="s">
-        <v>440</v>
+        <v>437</v>
       </c>
       <c r="D125" s="26" t="s">
         <v>6</v>
@@ -4452,7 +4484,7 @@
         <v>6</v>
       </c>
       <c r="I125" s="35" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="126" spans="1:9" ht="15" x14ac:dyDescent="0.15">
@@ -4469,7 +4501,7 @@
         <v>6</v>
       </c>
       <c r="I126" s="32" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="127" spans="1:9" ht="15" x14ac:dyDescent="0.15">
@@ -4477,16 +4509,16 @@
         <v>142</v>
       </c>
       <c r="B127" s="6" t="s">
+        <v>283</v>
+      </c>
+      <c r="E127" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="H127" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="I127" s="32" t="s">
         <v>284</v>
-      </c>
-      <c r="E127" s="19" t="s">
-        <v>6</v>
-      </c>
-      <c r="H127" s="19" t="s">
-        <v>6</v>
-      </c>
-      <c r="I127" s="32" t="s">
-        <v>285</v>
       </c>
     </row>
     <row r="128" spans="1:9" s="27" customFormat="1" ht="45" x14ac:dyDescent="0.15">
@@ -4494,7 +4526,7 @@
         <v>141</v>
       </c>
       <c r="B128" s="27" t="s">
-        <v>441</v>
+        <v>438</v>
       </c>
       <c r="D128" s="26" t="s">
         <v>6</v>
@@ -4506,7 +4538,7 @@
         <v>6</v>
       </c>
       <c r="I128" s="35" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="129" spans="1:9" ht="15" x14ac:dyDescent="0.15">
@@ -4523,7 +4555,7 @@
         <v>6</v>
       </c>
       <c r="I129" s="32" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="130" spans="1:9" ht="15" x14ac:dyDescent="0.15">
@@ -4531,7 +4563,7 @@
         <v>144</v>
       </c>
       <c r="B130" s="6" t="s">
-        <v>417</v>
+        <v>414</v>
       </c>
       <c r="E130" s="19" t="s">
         <v>6</v>
@@ -4540,7 +4572,7 @@
         <v>6</v>
       </c>
       <c r="I130" s="32" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="131" spans="1:9" ht="15" x14ac:dyDescent="0.15">
@@ -4557,7 +4589,7 @@
         <v>6</v>
       </c>
       <c r="I131" s="32" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="132" spans="1:9" ht="15" x14ac:dyDescent="0.15">
@@ -4574,7 +4606,7 @@
         <v>6</v>
       </c>
       <c r="I132" s="32" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="133" spans="1:9" ht="15" x14ac:dyDescent="0.15">
@@ -4591,7 +4623,7 @@
         <v>6</v>
       </c>
       <c r="I133" s="32" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="134" spans="1:9" ht="15" x14ac:dyDescent="0.15">
@@ -4599,7 +4631,7 @@
         <v>146</v>
       </c>
       <c r="B134" s="6" t="s">
-        <v>442</v>
+        <v>439</v>
       </c>
       <c r="D134" s="19" t="s">
         <v>6</v>
@@ -4608,7 +4640,7 @@
         <v>6</v>
       </c>
       <c r="I134" s="32" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="135" spans="1:9" ht="135" x14ac:dyDescent="0.15">
@@ -4625,7 +4657,7 @@
         <v>6</v>
       </c>
       <c r="I135" s="32" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="136" spans="1:9" ht="45" x14ac:dyDescent="0.15">
@@ -4633,19 +4665,19 @@
         <v>148</v>
       </c>
       <c r="B136" s="6" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C136" s="32" t="s">
+        <v>290</v>
+      </c>
+      <c r="D136" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="H136" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="I136" s="32" t="s">
         <v>291</v>
-      </c>
-      <c r="D136" s="19" t="s">
-        <v>6</v>
-      </c>
-      <c r="H136" s="19" t="s">
-        <v>6</v>
-      </c>
-      <c r="I136" s="32" t="s">
-        <v>292</v>
       </c>
     </row>
     <row r="137" spans="1:9" ht="30" x14ac:dyDescent="0.15">
@@ -4653,7 +4685,7 @@
         <v>149</v>
       </c>
       <c r="B137" s="6" t="s">
-        <v>443</v>
+        <v>440</v>
       </c>
       <c r="E137" s="19" t="s">
         <v>6</v>
@@ -4662,7 +4694,7 @@
         <v>6</v>
       </c>
       <c r="I137" s="32" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="138" spans="1:9" ht="75" x14ac:dyDescent="0.15">
@@ -4679,7 +4711,7 @@
         <v>6</v>
       </c>
       <c r="I138" s="32" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="139" spans="1:9" ht="15" x14ac:dyDescent="0.15">
@@ -4696,7 +4728,7 @@
         <v>6</v>
       </c>
       <c r="I139" s="32" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="140" spans="1:9" s="17" customFormat="1" ht="30" x14ac:dyDescent="0.15">
@@ -4704,7 +4736,7 @@
         <v>154</v>
       </c>
       <c r="B140" s="17" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="D140" s="21"/>
       <c r="E140" s="21"/>
@@ -4716,7 +4748,7 @@
         <v>6</v>
       </c>
       <c r="I140" s="33" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="141" spans="1:9" s="17" customFormat="1" ht="15" x14ac:dyDescent="0.15">
@@ -4724,7 +4756,7 @@
         <v>153</v>
       </c>
       <c r="B141" s="17" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="D141" s="21"/>
       <c r="E141" s="21"/>
@@ -4736,7 +4768,7 @@
         <v>6</v>
       </c>
       <c r="I141" s="33" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="142" spans="1:9" s="17" customFormat="1" ht="30" x14ac:dyDescent="0.15">
@@ -4744,7 +4776,7 @@
         <v>155</v>
       </c>
       <c r="B142" s="17" t="s">
-        <v>445</v>
+        <v>442</v>
       </c>
       <c r="D142" s="21"/>
       <c r="E142" s="21"/>
@@ -4756,7 +4788,7 @@
         <v>6</v>
       </c>
       <c r="I142" s="33" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="143" spans="1:9" ht="15" x14ac:dyDescent="0.15">
@@ -4764,7 +4796,7 @@
         <v>152</v>
       </c>
       <c r="B143" s="6" t="s">
-        <v>416</v>
+        <v>413</v>
       </c>
       <c r="D143" s="19" t="s">
         <v>6</v>
@@ -4773,7 +4805,7 @@
         <v>6</v>
       </c>
       <c r="I143" s="32" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="144" spans="1:9" s="27" customFormat="1" ht="60" x14ac:dyDescent="0.15">
@@ -4781,7 +4813,7 @@
         <v>156</v>
       </c>
       <c r="B144" s="27" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="D144" s="26" t="s">
         <v>6</v>
@@ -4793,7 +4825,7 @@
         <v>6</v>
       </c>
       <c r="I144" s="35" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="145" spans="1:9" ht="30" x14ac:dyDescent="0.15">
@@ -4810,7 +4842,7 @@
         <v>6</v>
       </c>
       <c r="I145" s="32" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="146" spans="1:9" s="27" customFormat="1" ht="15" x14ac:dyDescent="0.15">
@@ -4818,7 +4850,7 @@
         <v>158</v>
       </c>
       <c r="B146" s="27" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="D146" s="26" t="s">
         <v>6</v>
@@ -4830,7 +4862,7 @@
         <v>6</v>
       </c>
       <c r="I146" s="35" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="147" spans="1:9" ht="15" x14ac:dyDescent="0.15">
@@ -4847,7 +4879,7 @@
         <v>6</v>
       </c>
       <c r="I147" s="32" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="148" spans="1:9" ht="45" x14ac:dyDescent="0.15">
@@ -4855,7 +4887,7 @@
         <v>167</v>
       </c>
       <c r="B148" s="6" t="s">
-        <v>446</v>
+        <v>443</v>
       </c>
       <c r="E148" s="19" t="s">
         <v>6</v>
@@ -4864,7 +4896,7 @@
         <v>6</v>
       </c>
       <c r="I148" s="32" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="149" spans="1:9" s="27" customFormat="1" ht="30" x14ac:dyDescent="0.15">
@@ -4872,7 +4904,7 @@
         <v>165</v>
       </c>
       <c r="B149" s="27" t="s">
-        <v>447</v>
+        <v>444</v>
       </c>
       <c r="D149" s="26"/>
       <c r="E149" s="26" t="s">
@@ -4884,7 +4916,7 @@
         <v>6</v>
       </c>
       <c r="I149" s="35" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="150" spans="1:9" ht="15" x14ac:dyDescent="0.15">
@@ -4901,7 +4933,7 @@
         <v>6</v>
       </c>
       <c r="I150" s="32" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="151" spans="1:9" ht="15" x14ac:dyDescent="0.15">
@@ -4918,7 +4950,7 @@
         <v>6</v>
       </c>
       <c r="I151" s="32" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="152" spans="1:9" ht="30" x14ac:dyDescent="0.15">
@@ -4935,7 +4967,7 @@
         <v>6</v>
       </c>
       <c r="I152" s="32" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="153" spans="1:9" ht="15" x14ac:dyDescent="0.15">
@@ -4952,7 +4984,7 @@
         <v>6</v>
       </c>
       <c r="I153" s="32" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="154" spans="1:9" ht="45" x14ac:dyDescent="0.15">
@@ -4969,7 +5001,7 @@
         <v>6</v>
       </c>
       <c r="I154" s="32" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="155" spans="1:9" ht="15" x14ac:dyDescent="0.15">
@@ -4977,16 +5009,16 @@
         <v>189</v>
       </c>
       <c r="B155" s="6" t="s">
+        <v>308</v>
+      </c>
+      <c r="D155" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="H155" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="I155" s="32" t="s">
         <v>309</v>
-      </c>
-      <c r="D155" s="19" t="s">
-        <v>6</v>
-      </c>
-      <c r="H155" s="19" t="s">
-        <v>6</v>
-      </c>
-      <c r="I155" s="32" t="s">
-        <v>310</v>
       </c>
     </row>
     <row r="156" spans="1:9" s="17" customFormat="1" ht="60" x14ac:dyDescent="0.15">
@@ -4994,7 +5026,7 @@
         <v>193</v>
       </c>
       <c r="B156" s="17" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="C156" s="17" t="s">
         <v>35</v>
@@ -5009,7 +5041,7 @@
         <v>6</v>
       </c>
       <c r="I156" s="33" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="157" spans="1:9" ht="15" x14ac:dyDescent="0.15">
@@ -5026,7 +5058,7 @@
         <v>6</v>
       </c>
       <c r="I157" s="32" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="158" spans="1:9" s="27" customFormat="1" ht="30" x14ac:dyDescent="0.15">
@@ -5034,7 +5066,7 @@
         <v>187</v>
       </c>
       <c r="B158" s="27" t="s">
-        <v>448</v>
+        <v>445</v>
       </c>
       <c r="D158" s="26"/>
       <c r="E158" s="26" t="s">
@@ -5046,7 +5078,7 @@
         <v>6</v>
       </c>
       <c r="I158" s="35" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="159" spans="1:9" ht="45" x14ac:dyDescent="0.15">
@@ -5054,7 +5086,7 @@
         <v>186</v>
       </c>
       <c r="B159" s="6" t="s">
-        <v>449</v>
+        <v>446</v>
       </c>
       <c r="D159" s="19" t="s">
         <v>6</v>
@@ -5063,7 +5095,7 @@
         <v>6</v>
       </c>
       <c r="I159" s="32" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="160" spans="1:9" ht="15" x14ac:dyDescent="0.15">
@@ -5071,7 +5103,7 @@
         <v>185</v>
       </c>
       <c r="B160" s="6" t="s">
-        <v>450</v>
+        <v>447</v>
       </c>
       <c r="D160" s="19" t="s">
         <v>6</v>
@@ -5080,7 +5112,7 @@
         <v>6</v>
       </c>
       <c r="I160" s="32" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="161" spans="1:9" ht="15" x14ac:dyDescent="0.15">
@@ -5097,7 +5129,7 @@
         <v>6</v>
       </c>
       <c r="I161" s="32" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="162" spans="1:9" s="27" customFormat="1" ht="30" x14ac:dyDescent="0.15">
@@ -5105,7 +5137,7 @@
         <v>182</v>
       </c>
       <c r="B162" s="27" t="s">
-        <v>451</v>
+        <v>448</v>
       </c>
       <c r="C162" s="35"/>
       <c r="D162" s="26"/>
@@ -5118,7 +5150,7 @@
         <v>6</v>
       </c>
       <c r="I162" s="35" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="163" spans="1:9" ht="15" x14ac:dyDescent="0.15">
@@ -5132,7 +5164,7 @@
         <v>6</v>
       </c>
       <c r="I163" s="32" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="164" spans="1:9" ht="30" x14ac:dyDescent="0.15">
@@ -5146,7 +5178,7 @@
         <v>6</v>
       </c>
       <c r="I164" s="32" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="165" spans="1:9" ht="30" x14ac:dyDescent="0.15">
@@ -5154,13 +5186,13 @@
         <v>179</v>
       </c>
       <c r="B165" s="6" t="s">
+        <v>318</v>
+      </c>
+      <c r="E165" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="I165" s="32" t="s">
         <v>319</v>
-      </c>
-      <c r="E165" s="19" t="s">
-        <v>6</v>
-      </c>
-      <c r="I165" s="32" t="s">
-        <v>320</v>
       </c>
     </row>
     <row r="166" spans="1:9" ht="15" x14ac:dyDescent="0.15">
@@ -5174,7 +5206,7 @@
         <v>6</v>
       </c>
       <c r="I166" s="32" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="167" spans="1:9" s="27" customFormat="1" ht="30" x14ac:dyDescent="0.15">
@@ -5192,7 +5224,7 @@
       <c r="G167" s="47"/>
       <c r="H167" s="26"/>
       <c r="I167" s="35" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="168" spans="1:9" ht="30" x14ac:dyDescent="0.15">
@@ -5206,7 +5238,7 @@
         <v>6</v>
       </c>
       <c r="I168" s="32" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="169" spans="1:9" ht="15" x14ac:dyDescent="0.15">
@@ -5214,13 +5246,13 @@
         <v>174</v>
       </c>
       <c r="B169" s="6" t="s">
+        <v>323</v>
+      </c>
+      <c r="D169" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="I169" s="32" t="s">
         <v>324</v>
-      </c>
-      <c r="D169" s="19" t="s">
-        <v>6</v>
-      </c>
-      <c r="I169" s="32" t="s">
-        <v>325</v>
       </c>
     </row>
     <row r="170" spans="1:9" ht="15" x14ac:dyDescent="0.15">
@@ -5228,13 +5260,13 @@
         <v>173</v>
       </c>
       <c r="B170" s="6" t="s">
+        <v>325</v>
+      </c>
+      <c r="E170" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="I170" s="32" t="s">
         <v>326</v>
-      </c>
-      <c r="E170" s="19" t="s">
-        <v>6</v>
-      </c>
-      <c r="I170" s="32" t="s">
-        <v>327</v>
       </c>
     </row>
     <row r="171" spans="1:9" ht="30" x14ac:dyDescent="0.15">
@@ -5248,15 +5280,15 @@
         <v>6</v>
       </c>
       <c r="I171" s="32" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="172" spans="1:9" s="17" customFormat="1" ht="30" x14ac:dyDescent="0.15">
       <c r="A172" s="17" t="s">
+        <v>328</v>
+      </c>
+      <c r="B172" s="17" t="s">
         <v>329</v>
-      </c>
-      <c r="B172" s="17" t="s">
-        <v>330</v>
       </c>
       <c r="D172" s="21"/>
       <c r="E172" s="21"/>
@@ -5266,12 +5298,12 @@
       <c r="G172" s="48"/>
       <c r="H172" s="21"/>
       <c r="I172" s="33" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="173" spans="1:9" ht="15" x14ac:dyDescent="0.15">
       <c r="A173" s="6" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B173" s="6" t="s">
         <v>168</v>
@@ -5280,18 +5312,18 @@
         <v>6</v>
       </c>
       <c r="I173" s="32" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="174" spans="1:9" s="17" customFormat="1" ht="60" x14ac:dyDescent="0.15">
       <c r="A174" s="17" t="s">
+        <v>333</v>
+      </c>
+      <c r="B174" s="17" t="s">
         <v>334</v>
       </c>
-      <c r="B174" s="17" t="s">
-        <v>335</v>
-      </c>
       <c r="C174" s="17" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="D174" s="21"/>
       <c r="E174" s="21"/>
@@ -5301,12 +5333,12 @@
       <c r="G174" s="48"/>
       <c r="H174" s="21"/>
       <c r="I174" s="33" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="175" spans="1:9" ht="15" x14ac:dyDescent="0.15">
       <c r="A175" s="6" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="B175" s="6" t="s">
         <v>74</v>
@@ -5315,12 +5347,12 @@
         <v>6</v>
       </c>
       <c r="I175" s="32" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="176" spans="1:9" ht="15" x14ac:dyDescent="0.15">
       <c r="A176" s="6" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="B176" s="6" t="s">
         <v>116</v>
@@ -5329,12 +5361,12 @@
         <v>6</v>
       </c>
       <c r="I176" s="32" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="177" spans="1:9" s="27" customFormat="1" ht="15" x14ac:dyDescent="0.15">
       <c r="A177" s="27" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="B177" s="27" t="s">
         <v>28</v>
@@ -5347,15 +5379,15 @@
       <c r="G177" s="47"/>
       <c r="H177" s="26"/>
       <c r="I177" s="35" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="178" spans="1:9" s="17" customFormat="1" ht="30" x14ac:dyDescent="0.15">
       <c r="A178" s="17" t="s">
+        <v>342</v>
+      </c>
+      <c r="B178" s="17" t="s">
         <v>343</v>
-      </c>
-      <c r="B178" s="17" t="s">
-        <v>344</v>
       </c>
       <c r="D178" s="21"/>
       <c r="E178" s="21" t="s">
@@ -5365,26 +5397,26 @@
       <c r="G178" s="48"/>
       <c r="H178" s="21"/>
       <c r="I178" s="33" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
     </row>
     <row r="179" spans="1:9" ht="30" x14ac:dyDescent="0.15">
       <c r="A179" s="6" t="s">
+        <v>345</v>
+      </c>
+      <c r="B179" s="6" t="s">
         <v>346</v>
       </c>
-      <c r="B179" s="6" t="s">
+      <c r="E179" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="I179" s="32" t="s">
         <v>347</v>
-      </c>
-      <c r="E179" s="19" t="s">
-        <v>6</v>
-      </c>
-      <c r="I179" s="32" t="s">
-        <v>348</v>
       </c>
     </row>
     <row r="180" spans="1:9" s="27" customFormat="1" ht="60" x14ac:dyDescent="0.15">
       <c r="A180" s="27" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="B180" s="27" t="s">
         <v>15</v>
@@ -5397,15 +5429,15 @@
       <c r="G180" s="47"/>
       <c r="H180" s="26"/>
       <c r="I180" s="35" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
     </row>
     <row r="181" spans="1:9" s="17" customFormat="1" ht="45" x14ac:dyDescent="0.15">
       <c r="A181" s="17" t="s">
+        <v>350</v>
+      </c>
+      <c r="B181" s="17" t="s">
         <v>351</v>
-      </c>
-      <c r="B181" s="17" t="s">
-        <v>352</v>
       </c>
       <c r="D181" s="21"/>
       <c r="E181" s="21"/>
@@ -5415,12 +5447,12 @@
       <c r="G181" s="48"/>
       <c r="H181" s="21"/>
       <c r="I181" s="33" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
     </row>
     <row r="182" spans="1:9" ht="30" x14ac:dyDescent="0.15">
       <c r="A182" s="6" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B182" s="6" t="s">
         <v>15</v>
@@ -5429,26 +5461,26 @@
         <v>6</v>
       </c>
       <c r="I182" s="32" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="183" spans="1:9" ht="15" x14ac:dyDescent="0.15">
       <c r="A183" s="6" t="s">
+        <v>355</v>
+      </c>
+      <c r="B183" s="6" t="s">
         <v>356</v>
       </c>
-      <c r="B183" s="6" t="s">
+      <c r="E183" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="I183" s="32" t="s">
         <v>357</v>
-      </c>
-      <c r="E183" s="19" t="s">
-        <v>6</v>
-      </c>
-      <c r="I183" s="32" t="s">
-        <v>358</v>
       </c>
     </row>
     <row r="184" spans="1:9" ht="15" x14ac:dyDescent="0.15">
       <c r="A184" s="6" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="B184" s="6" t="s">
         <v>76</v>
@@ -5457,21 +5489,21 @@
         <v>6</v>
       </c>
       <c r="I184" s="32" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="185" spans="1:9" ht="90" x14ac:dyDescent="0.15">
       <c r="A185" s="6" t="s">
+        <v>360</v>
+      </c>
+      <c r="B185" s="6" t="s">
         <v>361</v>
       </c>
-      <c r="B185" s="6" t="s">
+      <c r="F185" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="I185" s="32" t="s">
         <v>362</v>
-      </c>
-      <c r="F185" s="19" t="s">
-        <v>6</v>
-      </c>
-      <c r="I185" s="32" t="s">
-        <v>363</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feb 2 2024 update
</commit_message>
<xml_diff>
--- a/SQL/leetcode - sql.xlsx
+++ b/SQL/leetcode - sql.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zw/Documents/Github/LeetCode_Practice/SQL/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A36A445A-876E-1445-9534-D3C684C6306C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13113862-FADE-7C47-86D1-51991B14AC41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="945" uniqueCount="462">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="950" uniqueCount="462">
   <si>
     <t>Title</t>
   </si>
@@ -702,9 +702,6 @@
   </si>
   <si>
     <t>Cal &amp; Not In</t>
-  </si>
-  <si>
-    <t>想通了其实就很简单，只需要保证两点：1. Customer的product是在Product表里面的 2.从Customer表中计算的product数量和从Product表中抽出来的数量一致</t>
   </si>
   <si>
     <t>很简单的group by计数题</t>
@@ -1600,6 +1597,11 @@
     <t>求余数：
 1. mod(a,b) -&gt; a/b的余数
 2. a%b -&gt; a/b的余数</t>
+  </si>
+  <si>
+    <t>想通了其实就很简单，只需要保证两点：
+1. Customer的product是在Product表里面的 
+2.从Customer表中计算的product数量和从Product表中抽出来的数量一致</t>
   </si>
 </sst>
 </file>
@@ -2103,9 +2105,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1C70A3A-EB9B-3540-8C26-B9C443B2B647}">
   <dimension ref="A1:I185"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="112" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="112" zoomScaleNormal="120" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A49" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G50" sqref="G50"/>
+      <selection pane="bottomLeft" activeCell="G57" sqref="G57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="28" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -2169,10 +2171,10 @@
         <v>1</v>
       </c>
       <c r="G6" s="45" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="H6" s="12" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="I6" s="11" t="s">
         <v>194</v>
@@ -2219,7 +2221,7 @@
         <v>6</v>
       </c>
       <c r="I8" s="4" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
     </row>
     <row r="9" spans="1:9" s="27" customFormat="1" ht="76" thickBot="1" x14ac:dyDescent="0.2">
@@ -2242,7 +2244,7 @@
         <v>6</v>
       </c>
       <c r="I9" s="25" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="91" thickBot="1" x14ac:dyDescent="0.2">
@@ -2263,7 +2265,7 @@
         <v>6</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
     </row>
     <row r="11" spans="1:9" s="14" customFormat="1" ht="61" thickBot="1" x14ac:dyDescent="0.2">
@@ -2286,7 +2288,7 @@
         <v>6</v>
       </c>
       <c r="I11" s="4" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.2">
@@ -2336,7 +2338,7 @@
         <v>21</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C14" s="2"/>
       <c r="D14" s="19" t="s">
@@ -2349,7 +2351,7 @@
         <v>6</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="31" thickBot="1" x14ac:dyDescent="0.2">
@@ -2370,7 +2372,7 @@
         <v>6</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="31" thickBot="1" x14ac:dyDescent="0.2">
@@ -2416,7 +2418,7 @@
         <v>6</v>
       </c>
       <c r="I17" s="25" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
     </row>
     <row r="18" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.2">
@@ -2447,7 +2449,7 @@
         <v>29</v>
       </c>
       <c r="B19" s="16" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="C19" s="16"/>
       <c r="D19" s="21"/>
@@ -2462,7 +2464,7 @@
         <v>6</v>
       </c>
       <c r="I19" s="29" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="20" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.2">
@@ -2491,7 +2493,7 @@
         <v>31</v>
       </c>
       <c r="B21" s="41" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="C21" s="2"/>
       <c r="D21" s="19" t="s">
@@ -2504,7 +2506,7 @@
         <v>6</v>
       </c>
       <c r="I21" s="40" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
     </row>
     <row r="22" spans="1:9" s="27" customFormat="1" ht="46" thickBot="1" x14ac:dyDescent="0.2">
@@ -2512,7 +2514,7 @@
         <v>32</v>
       </c>
       <c r="B22" s="50" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="C22" s="25"/>
       <c r="D22" s="26"/>
@@ -2527,7 +2529,7 @@
         <v>6</v>
       </c>
       <c r="I22" s="51" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
     </row>
     <row r="23" spans="1:9" ht="31" thickBot="1" x14ac:dyDescent="0.2">
@@ -2548,7 +2550,7 @@
         <v>6</v>
       </c>
       <c r="I23" s="40" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="24" spans="1:9" s="17" customFormat="1" ht="91" thickBot="1" x14ac:dyDescent="0.2">
@@ -2573,7 +2575,7 @@
         <v>6</v>
       </c>
       <c r="I24" s="29" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="25" spans="1:9" s="14" customFormat="1" ht="46" thickBot="1" x14ac:dyDescent="0.2">
@@ -2596,7 +2598,7 @@
         <v>6</v>
       </c>
       <c r="I25" s="53" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
     </row>
     <row r="26" spans="1:9" s="17" customFormat="1" ht="409.6" thickBot="1" x14ac:dyDescent="0.2">
@@ -2604,7 +2606,7 @@
         <v>35</v>
       </c>
       <c r="B26" s="16" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="C26" s="28" t="s">
         <v>34</v>
@@ -2621,7 +2623,7 @@
         <v>6</v>
       </c>
       <c r="I26" s="29" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
     <row r="27" spans="1:9" ht="31" thickBot="1" x14ac:dyDescent="0.2">
@@ -2629,7 +2631,7 @@
         <v>37</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="C27" s="2"/>
       <c r="E27" s="19" t="s">
@@ -2642,7 +2644,7 @@
         <v>6</v>
       </c>
       <c r="I27" s="24" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
     </row>
     <row r="28" spans="1:9" ht="46" thickBot="1" x14ac:dyDescent="0.2">
@@ -2650,7 +2652,7 @@
         <v>8</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="C28" s="1"/>
       <c r="D28" s="19" t="s">
@@ -2663,7 +2665,7 @@
         <v>6</v>
       </c>
       <c r="I28" s="32" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="29" spans="1:9" ht="210" x14ac:dyDescent="0.15">
@@ -2683,7 +2685,7 @@
         <v>6</v>
       </c>
       <c r="I29" s="32" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="30" spans="1:9" s="17" customFormat="1" ht="255" x14ac:dyDescent="0.15">
@@ -2691,7 +2693,7 @@
         <v>40</v>
       </c>
       <c r="B30" s="17" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="D30" s="21"/>
       <c r="E30" s="21"/>
@@ -2745,7 +2747,7 @@
         <v>6</v>
       </c>
       <c r="I32" s="32" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="33" spans="1:9" ht="46" thickBot="1" x14ac:dyDescent="0.2">
@@ -2765,7 +2767,7 @@
         <v>6</v>
       </c>
       <c r="I33" s="32" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="34" spans="1:9" ht="15" x14ac:dyDescent="0.15">
@@ -2847,7 +2849,7 @@
         <v>6</v>
       </c>
       <c r="I37" s="35" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
     </row>
     <row r="38" spans="1:9" s="17" customFormat="1" ht="180" x14ac:dyDescent="0.15">
@@ -2872,7 +2874,7 @@
         <v>6</v>
       </c>
       <c r="I38" s="33" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
     </row>
     <row r="39" spans="1:9" ht="30" x14ac:dyDescent="0.15">
@@ -2880,7 +2882,7 @@
         <v>50</v>
       </c>
       <c r="B39" s="6" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="E39" s="19" t="s">
         <v>6</v>
@@ -2915,7 +2917,7 @@
         <v>6</v>
       </c>
       <c r="I40" s="32" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
     </row>
     <row r="41" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.2">
@@ -2923,7 +2925,7 @@
         <v>51</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="D41" s="19" t="s">
         <v>6</v>
@@ -2935,7 +2937,7 @@
         <v>6</v>
       </c>
       <c r="I41" s="32" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
     </row>
     <row r="42" spans="1:9" ht="30" x14ac:dyDescent="0.15">
@@ -2943,7 +2945,7 @@
         <v>52</v>
       </c>
       <c r="B42" s="6" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="E42" s="19" t="s">
         <v>6</v>
@@ -2955,7 +2957,7 @@
         <v>6</v>
       </c>
       <c r="I42" s="32" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="43" spans="1:9" ht="30" x14ac:dyDescent="0.15">
@@ -2963,7 +2965,7 @@
         <v>53</v>
       </c>
       <c r="B43" s="6" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="D43" s="19" t="s">
         <v>6</v>
@@ -2983,7 +2985,7 @@
         <v>160</v>
       </c>
       <c r="B44" s="27" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="C44" s="27" t="s">
         <v>161</v>
@@ -3000,7 +3002,7 @@
         <v>6</v>
       </c>
       <c r="I44" s="35" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
     </row>
     <row r="45" spans="1:9" ht="15" x14ac:dyDescent="0.15">
@@ -3051,7 +3053,7 @@
         <v>132</v>
       </c>
       <c r="B47" s="6" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="C47" s="6" t="s">
         <v>73</v>
@@ -3066,7 +3068,7 @@
         <v>6</v>
       </c>
       <c r="I47" s="32" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
     </row>
     <row r="48" spans="1:9" s="17" customFormat="1" ht="75" x14ac:dyDescent="0.15">
@@ -3088,7 +3090,7 @@
         <v>6</v>
       </c>
       <c r="I48" s="33" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
     </row>
     <row r="49" spans="1:9" s="14" customFormat="1" ht="30" x14ac:dyDescent="0.15">
@@ -3130,7 +3132,7 @@
         <v>6</v>
       </c>
       <c r="I50" s="32" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
     </row>
     <row r="51" spans="1:9" s="17" customFormat="1" ht="60" x14ac:dyDescent="0.15">
@@ -3152,7 +3154,7 @@
         <v>6</v>
       </c>
       <c r="I51" s="33" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="52" spans="1:9" s="27" customFormat="1" ht="15" x14ac:dyDescent="0.15">
@@ -3160,14 +3162,16 @@
         <v>55</v>
       </c>
       <c r="B52" s="27" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="D52" s="26" t="s">
         <v>6</v>
       </c>
       <c r="E52" s="26"/>
       <c r="F52" s="26"/>
-      <c r="G52" s="47"/>
+      <c r="G52" s="47" t="s">
+        <v>6</v>
+      </c>
       <c r="H52" s="26" t="s">
         <v>6</v>
       </c>
@@ -3185,11 +3189,14 @@
       <c r="E53" s="19" t="s">
         <v>6</v>
       </c>
+      <c r="G53" s="44" t="s">
+        <v>6</v>
+      </c>
       <c r="H53" s="19" t="s">
         <v>6</v>
       </c>
       <c r="I53" s="32" t="s">
-        <v>221</v>
+        <v>461</v>
       </c>
     </row>
     <row r="54" spans="1:9" ht="15" x14ac:dyDescent="0.15">
@@ -3202,11 +3209,14 @@
       <c r="D54" s="19" t="s">
         <v>6</v>
       </c>
+      <c r="G54" s="44" t="s">
+        <v>6</v>
+      </c>
       <c r="H54" s="19" t="s">
         <v>6</v>
       </c>
       <c r="I54" s="32" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="55" spans="1:9" ht="15" x14ac:dyDescent="0.15">
@@ -3219,11 +3229,14 @@
       <c r="D55" s="19" t="s">
         <v>6</v>
       </c>
+      <c r="G55" s="44" t="s">
+        <v>6</v>
+      </c>
       <c r="H55" s="19" t="s">
         <v>6</v>
       </c>
       <c r="I55" s="32" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="56" spans="1:9" ht="15" x14ac:dyDescent="0.15">
@@ -3236,11 +3249,14 @@
       <c r="D56" s="19" t="s">
         <v>6</v>
       </c>
+      <c r="G56" s="44" t="s">
+        <v>6</v>
+      </c>
       <c r="H56" s="19" t="s">
         <v>6</v>
       </c>
       <c r="I56" s="32" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="57" spans="1:9" ht="45" x14ac:dyDescent="0.15">
@@ -3248,16 +3264,16 @@
         <v>61</v>
       </c>
       <c r="B57" s="6" t="s">
+        <v>393</v>
+      </c>
+      <c r="E57" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="H57" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="I57" s="32" t="s">
         <v>394</v>
-      </c>
-      <c r="E57" s="19" t="s">
-        <v>6</v>
-      </c>
-      <c r="H57" s="19" t="s">
-        <v>6</v>
-      </c>
-      <c r="I57" s="32" t="s">
-        <v>395</v>
       </c>
     </row>
     <row r="58" spans="1:9" ht="15" x14ac:dyDescent="0.15">
@@ -3274,7 +3290,7 @@
         <v>6</v>
       </c>
       <c r="I58" s="32" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="59" spans="1:9" ht="30" x14ac:dyDescent="0.15">
@@ -3294,7 +3310,7 @@
         <v>6</v>
       </c>
       <c r="I59" s="32" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="60" spans="1:9" ht="45" x14ac:dyDescent="0.15">
@@ -3311,7 +3327,7 @@
         <v>6</v>
       </c>
       <c r="I60" s="32" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
     </row>
     <row r="61" spans="1:9" ht="15" x14ac:dyDescent="0.15">
@@ -3331,7 +3347,7 @@
         <v>6</v>
       </c>
       <c r="I61" s="32" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
     </row>
     <row r="62" spans="1:9" s="14" customFormat="1" ht="45" x14ac:dyDescent="0.15">
@@ -3339,7 +3355,7 @@
         <v>66</v>
       </c>
       <c r="B62" s="14" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="D62" s="20" t="s">
         <v>6</v>
@@ -3351,7 +3367,7 @@
         <v>6</v>
       </c>
       <c r="I62" s="34" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="63" spans="1:9" ht="46" thickBot="1" x14ac:dyDescent="0.2">
@@ -3359,7 +3375,7 @@
         <v>67</v>
       </c>
       <c r="B63" s="6" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="D63" s="19" t="s">
         <v>6</v>
@@ -3368,7 +3384,7 @@
         <v>6</v>
       </c>
       <c r="I63" s="32" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
     </row>
     <row r="64" spans="1:9" ht="31" thickBot="1" x14ac:dyDescent="0.2">
@@ -3376,7 +3392,7 @@
         <v>68</v>
       </c>
       <c r="B64" s="41" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="C64" s="2"/>
       <c r="F64" s="19" t="s">
@@ -3386,7 +3402,7 @@
         <v>6</v>
       </c>
       <c r="I64" s="40" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="65" spans="1:9" s="14" customFormat="1" ht="105" x14ac:dyDescent="0.15">
@@ -3394,7 +3410,7 @@
         <v>69</v>
       </c>
       <c r="B65" s="14" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="D65" s="20"/>
       <c r="E65" s="20" t="s">
@@ -3406,7 +3422,7 @@
         <v>6</v>
       </c>
       <c r="I65" s="34" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="66" spans="1:9" ht="15" x14ac:dyDescent="0.15">
@@ -3414,7 +3430,7 @@
         <v>70</v>
       </c>
       <c r="B66" s="6" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="E66" s="19" t="s">
         <v>6</v>
@@ -3423,7 +3439,7 @@
         <v>6</v>
       </c>
       <c r="I66" s="32" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="67" spans="1:9" ht="15" x14ac:dyDescent="0.15">
@@ -3440,7 +3456,7 @@
         <v>6</v>
       </c>
       <c r="I67" s="32" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="68" spans="1:9" ht="15" x14ac:dyDescent="0.15">
@@ -3457,7 +3473,7 @@
         <v>6</v>
       </c>
       <c r="I68" s="32" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="69" spans="1:9" ht="30" x14ac:dyDescent="0.15">
@@ -3477,7 +3493,7 @@
         <v>6</v>
       </c>
       <c r="I69" s="32" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="70" spans="1:9" s="17" customFormat="1" ht="90" x14ac:dyDescent="0.15">
@@ -3485,7 +3501,7 @@
         <v>75</v>
       </c>
       <c r="B70" s="17" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D70" s="21"/>
       <c r="E70" s="21"/>
@@ -3497,7 +3513,7 @@
         <v>6</v>
       </c>
       <c r="I70" s="33" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.15">
@@ -3514,7 +3530,7 @@
         <v>6</v>
       </c>
       <c r="I71" s="6" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="72" spans="1:9" ht="30" x14ac:dyDescent="0.15">
@@ -3531,7 +3547,7 @@
         <v>6</v>
       </c>
       <c r="I72" s="32" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="73" spans="1:9" ht="30" x14ac:dyDescent="0.15">
@@ -3548,7 +3564,7 @@
         <v>6</v>
       </c>
       <c r="I73" s="32" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="74" spans="1:9" ht="15" x14ac:dyDescent="0.15">
@@ -3565,7 +3581,7 @@
         <v>6</v>
       </c>
       <c r="I74" s="32" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="75" spans="1:9" s="14" customFormat="1" ht="75" x14ac:dyDescent="0.15">
@@ -3585,7 +3601,7 @@
         <v>6</v>
       </c>
       <c r="I75" s="34" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
     </row>
     <row r="76" spans="1:9" ht="60" x14ac:dyDescent="0.15">
@@ -3602,7 +3618,7 @@
         <v>6</v>
       </c>
       <c r="I76" s="32" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
     </row>
     <row r="77" spans="1:9" ht="30" x14ac:dyDescent="0.15">
@@ -3610,7 +3626,7 @@
         <v>85</v>
       </c>
       <c r="B77" s="6" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="F77" s="19" t="s">
         <v>6</v>
@@ -3619,7 +3635,7 @@
         <v>6</v>
       </c>
       <c r="I77" s="32" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="78" spans="1:9" ht="30" x14ac:dyDescent="0.15">
@@ -3627,7 +3643,7 @@
         <v>86</v>
       </c>
       <c r="B78" s="6" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="E78" s="19" t="s">
         <v>6</v>
@@ -3636,7 +3652,7 @@
         <v>6</v>
       </c>
       <c r="I78" s="32" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="79" spans="1:9" ht="15" x14ac:dyDescent="0.15">
@@ -3644,7 +3660,7 @@
         <v>87</v>
       </c>
       <c r="B79" s="6" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="D79" s="19" t="s">
         <v>6</v>
@@ -3653,7 +3669,7 @@
         <v>6</v>
       </c>
       <c r="I79" s="32" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="80" spans="1:9" ht="45" x14ac:dyDescent="0.15">
@@ -3661,7 +3677,7 @@
         <v>88</v>
       </c>
       <c r="B80" s="6" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="E80" s="19" t="s">
         <v>6</v>
@@ -3670,7 +3686,7 @@
         <v>6</v>
       </c>
       <c r="I80" s="32" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="81" spans="1:9" ht="30" x14ac:dyDescent="0.15">
@@ -3678,7 +3694,7 @@
         <v>89</v>
       </c>
       <c r="B81" s="6" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="D81" s="19" t="s">
         <v>6</v>
@@ -3687,7 +3703,7 @@
         <v>6</v>
       </c>
       <c r="I81" s="32" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="82" spans="1:9" ht="15" x14ac:dyDescent="0.15">
@@ -3695,7 +3711,7 @@
         <v>90</v>
       </c>
       <c r="B82" s="6" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="E82" s="19" t="s">
         <v>6</v>
@@ -3704,7 +3720,7 @@
         <v>6</v>
       </c>
       <c r="I82" s="32" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="83" spans="1:9" ht="45" x14ac:dyDescent="0.15">
@@ -3712,7 +3728,7 @@
         <v>91</v>
       </c>
       <c r="B83" s="6" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="F83" s="19" t="s">
         <v>6</v>
@@ -3721,7 +3737,7 @@
         <v>6</v>
       </c>
       <c r="I83" s="32" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="84" spans="1:9" ht="15" x14ac:dyDescent="0.15">
@@ -3729,7 +3745,7 @@
         <v>92</v>
       </c>
       <c r="B84" s="6" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="E84" s="19" t="s">
         <v>6</v>
@@ -3738,7 +3754,7 @@
         <v>6</v>
       </c>
       <c r="I84" s="32" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="85" spans="1:9" s="17" customFormat="1" ht="45" x14ac:dyDescent="0.15">
@@ -3746,7 +3762,7 @@
         <v>93</v>
       </c>
       <c r="B85" s="17" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="D85" s="21"/>
       <c r="E85" s="21" t="s">
@@ -3758,7 +3774,7 @@
         <v>6</v>
       </c>
       <c r="I85" s="33" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="86" spans="1:9" ht="15" x14ac:dyDescent="0.15">
@@ -3766,7 +3782,7 @@
         <v>94</v>
       </c>
       <c r="B86" s="6" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="D86" s="19" t="s">
         <v>6</v>
@@ -3775,7 +3791,7 @@
         <v>6</v>
       </c>
       <c r="I86" s="32" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="87" spans="1:9" ht="15" x14ac:dyDescent="0.15">
@@ -3783,7 +3799,7 @@
         <v>95</v>
       </c>
       <c r="B87" s="6" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="E87" s="19" t="s">
         <v>6</v>
@@ -3792,7 +3808,7 @@
         <v>6</v>
       </c>
       <c r="I87" s="32" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="88" spans="1:9" s="17" customFormat="1" ht="150" x14ac:dyDescent="0.15">
@@ -3800,7 +3816,7 @@
         <v>98</v>
       </c>
       <c r="B88" s="17" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="C88" s="33"/>
       <c r="D88" s="21"/>
@@ -3813,7 +3829,7 @@
         <v>6</v>
       </c>
       <c r="I88" s="33" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
     </row>
     <row r="89" spans="1:9" ht="15" x14ac:dyDescent="0.15">
@@ -3830,7 +3846,7 @@
         <v>6</v>
       </c>
       <c r="I89" s="32" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="90" spans="1:9" ht="15" x14ac:dyDescent="0.15">
@@ -3847,7 +3863,7 @@
         <v>6</v>
       </c>
       <c r="I90" s="32" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="91" spans="1:9" ht="15" x14ac:dyDescent="0.15">
@@ -3855,7 +3871,7 @@
         <v>99</v>
       </c>
       <c r="B91" s="6" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="E91" s="19" t="s">
         <v>6</v>
@@ -3864,7 +3880,7 @@
         <v>6</v>
       </c>
       <c r="I91" s="32" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="92" spans="1:9" ht="15" x14ac:dyDescent="0.15">
@@ -3872,7 +3888,7 @@
         <v>100</v>
       </c>
       <c r="B92" s="6" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="E92" s="19" t="s">
         <v>6</v>
@@ -3881,7 +3897,7 @@
         <v>6</v>
       </c>
       <c r="I92" s="32" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="93" spans="1:9" s="14" customFormat="1" ht="75" x14ac:dyDescent="0.15">
@@ -3901,7 +3917,7 @@
         <v>6</v>
       </c>
       <c r="I93" s="34" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="94" spans="1:9" ht="15" x14ac:dyDescent="0.15">
@@ -3921,7 +3937,7 @@
         <v>6</v>
       </c>
       <c r="I94" s="32" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="95" spans="1:9" ht="30" x14ac:dyDescent="0.15">
@@ -3929,7 +3945,7 @@
         <v>103</v>
       </c>
       <c r="B95" s="6" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="D95" s="19" t="s">
         <v>6</v>
@@ -3938,7 +3954,7 @@
         <v>6</v>
       </c>
       <c r="I95" s="32" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
     </row>
     <row r="96" spans="1:9" s="27" customFormat="1" ht="60" x14ac:dyDescent="0.15">
@@ -3946,7 +3962,7 @@
         <v>104</v>
       </c>
       <c r="B96" s="27" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="D96" s="26" t="s">
         <v>6</v>
@@ -3958,7 +3974,7 @@
         <v>6</v>
       </c>
       <c r="I96" s="35" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="97" spans="1:9" ht="15" x14ac:dyDescent="0.15">
@@ -3966,7 +3982,7 @@
         <v>105</v>
       </c>
       <c r="B97" s="6" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="E97" s="19" t="s">
         <v>6</v>
@@ -3975,7 +3991,7 @@
         <v>6</v>
       </c>
       <c r="I97" s="32" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="98" spans="1:9" s="27" customFormat="1" ht="45" x14ac:dyDescent="0.15">
@@ -3983,7 +3999,7 @@
         <v>106</v>
       </c>
       <c r="B98" s="27" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="D98" s="26"/>
       <c r="E98" s="26" t="s">
@@ -3995,7 +4011,7 @@
         <v>6</v>
       </c>
       <c r="I98" s="35" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="99" spans="1:9" ht="45" x14ac:dyDescent="0.15">
@@ -4003,7 +4019,7 @@
         <v>107</v>
       </c>
       <c r="B99" s="6" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="D99" s="19" t="s">
         <v>6</v>
@@ -4012,7 +4028,7 @@
         <v>6</v>
       </c>
       <c r="I99" s="32" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="100" spans="1:9" ht="15" x14ac:dyDescent="0.15">
@@ -4029,7 +4045,7 @@
         <v>6</v>
       </c>
       <c r="I100" s="32" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="101" spans="1:9" s="17" customFormat="1" ht="180" x14ac:dyDescent="0.15">
@@ -4037,7 +4053,7 @@
         <v>112</v>
       </c>
       <c r="B101" s="17" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="D101" s="21"/>
       <c r="E101" s="21"/>
@@ -4049,7 +4065,7 @@
         <v>6</v>
       </c>
       <c r="I101" s="33" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="102" spans="1:9" ht="15" x14ac:dyDescent="0.15">
@@ -4066,7 +4082,7 @@
         <v>6</v>
       </c>
       <c r="I102" s="32" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="103" spans="1:9" ht="15" x14ac:dyDescent="0.15">
@@ -4074,7 +4090,7 @@
         <v>110</v>
       </c>
       <c r="B103" s="6" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="D103" s="19" t="s">
         <v>6</v>
@@ -4083,7 +4099,7 @@
         <v>6</v>
       </c>
       <c r="I103" s="32" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="104" spans="1:9" ht="60" x14ac:dyDescent="0.15">
@@ -4091,7 +4107,7 @@
         <v>113</v>
       </c>
       <c r="B104" s="6" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="E104" s="19" t="s">
         <v>6</v>
@@ -4100,7 +4116,7 @@
         <v>6</v>
       </c>
       <c r="I104" s="32" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="105" spans="1:9" ht="45" x14ac:dyDescent="0.15">
@@ -4108,16 +4124,16 @@
         <v>115</v>
       </c>
       <c r="B105" s="6" t="s">
+        <v>425</v>
+      </c>
+      <c r="E105" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="H105" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="I105" s="32" t="s">
         <v>426</v>
-      </c>
-      <c r="E105" s="19" t="s">
-        <v>6</v>
-      </c>
-      <c r="H105" s="19" t="s">
-        <v>6</v>
-      </c>
-      <c r="I105" s="32" t="s">
-        <v>427</v>
       </c>
     </row>
     <row r="106" spans="1:9" s="27" customFormat="1" ht="90" x14ac:dyDescent="0.15">
@@ -4125,7 +4141,7 @@
         <v>118</v>
       </c>
       <c r="B106" s="27" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="D106" s="26"/>
       <c r="E106" s="26"/>
@@ -4137,7 +4153,7 @@
         <v>6</v>
       </c>
       <c r="I106" s="35" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="107" spans="1:9" ht="15" x14ac:dyDescent="0.15">
@@ -4154,7 +4170,7 @@
         <v>6</v>
       </c>
       <c r="I107" s="32" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="108" spans="1:9" s="17" customFormat="1" ht="45" x14ac:dyDescent="0.15">
@@ -4162,7 +4178,7 @@
         <v>119</v>
       </c>
       <c r="B108" s="17" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="D108" s="21"/>
       <c r="E108" s="21"/>
@@ -4174,7 +4190,7 @@
         <v>6</v>
       </c>
       <c r="I108" s="33" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="109" spans="1:9" ht="15" x14ac:dyDescent="0.15">
@@ -4182,7 +4198,7 @@
         <v>120</v>
       </c>
       <c r="B109" s="6" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="E109" s="19" t="s">
         <v>6</v>
@@ -4191,7 +4207,7 @@
         <v>6</v>
       </c>
       <c r="I109" s="32" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="110" spans="1:9" ht="60" x14ac:dyDescent="0.15">
@@ -4208,7 +4224,7 @@
         <v>6</v>
       </c>
       <c r="I110" s="32" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="111" spans="1:9" ht="15" x14ac:dyDescent="0.15">
@@ -4225,7 +4241,7 @@
         <v>6</v>
       </c>
       <c r="I111" s="32" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="112" spans="1:9" s="14" customFormat="1" ht="46" x14ac:dyDescent="0.2">
@@ -4233,7 +4249,7 @@
         <v>124</v>
       </c>
       <c r="B112" s="42" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C112" s="14" t="s">
         <v>121</v>
@@ -4248,7 +4264,7 @@
         <v>6</v>
       </c>
       <c r="I112" s="34" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="113" spans="1:9" ht="15" x14ac:dyDescent="0.15">
@@ -4265,7 +4281,7 @@
         <v>6</v>
       </c>
       <c r="I113" s="32" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="114" spans="1:9" ht="30" x14ac:dyDescent="0.15">
@@ -4273,7 +4289,7 @@
         <v>125</v>
       </c>
       <c r="B114" s="6" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="D114" s="19" t="s">
         <v>6</v>
@@ -4282,7 +4298,7 @@
         <v>6</v>
       </c>
       <c r="I114" s="32" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="115" spans="1:9" s="17" customFormat="1" ht="30" x14ac:dyDescent="0.15">
@@ -4290,7 +4306,7 @@
         <v>126</v>
       </c>
       <c r="B115" s="17" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="D115" s="21"/>
       <c r="E115" s="21" t="s">
@@ -4302,7 +4318,7 @@
         <v>6</v>
       </c>
       <c r="I115" s="33" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="116" spans="1:9" ht="15" x14ac:dyDescent="0.15">
@@ -4310,7 +4326,7 @@
         <v>127</v>
       </c>
       <c r="B116" s="6" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="E116" s="19" t="s">
         <v>6</v>
@@ -4319,7 +4335,7 @@
         <v>6</v>
       </c>
       <c r="I116" s="32" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="117" spans="1:9" s="27" customFormat="1" ht="30" x14ac:dyDescent="0.15">
@@ -4327,7 +4343,7 @@
         <v>128</v>
       </c>
       <c r="B117" s="27" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="D117" s="26"/>
       <c r="E117" s="26" t="s">
@@ -4339,7 +4355,7 @@
         <v>6</v>
       </c>
       <c r="I117" s="35" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="118" spans="1:9" ht="45" x14ac:dyDescent="0.15">
@@ -4356,7 +4372,7 @@
         <v>6</v>
       </c>
       <c r="I118" s="32" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="119" spans="1:9" ht="15" x14ac:dyDescent="0.15">
@@ -4364,7 +4380,7 @@
         <v>130</v>
       </c>
       <c r="B119" s="6" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="E119" s="19" t="s">
         <v>6</v>
@@ -4373,7 +4389,7 @@
         <v>6</v>
       </c>
       <c r="I119" s="32" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="120" spans="1:9" s="17" customFormat="1" ht="15" x14ac:dyDescent="0.15">
@@ -4381,7 +4397,7 @@
         <v>136</v>
       </c>
       <c r="B120" s="17" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="D120" s="21"/>
       <c r="E120" s="21"/>
@@ -4393,7 +4409,7 @@
         <v>6</v>
       </c>
       <c r="I120" s="33" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="121" spans="1:9" s="27" customFormat="1" ht="60" x14ac:dyDescent="0.15">
@@ -4401,7 +4417,7 @@
         <v>133</v>
       </c>
       <c r="B121" s="27" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="D121" s="26" t="s">
         <v>6</v>
@@ -4413,7 +4429,7 @@
         <v>6</v>
       </c>
       <c r="I121" s="35" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="122" spans="1:9" ht="15" x14ac:dyDescent="0.15">
@@ -4421,16 +4437,16 @@
         <v>135</v>
       </c>
       <c r="B122" s="6" t="s">
+        <v>275</v>
+      </c>
+      <c r="D122" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="H122" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="I122" s="32" t="s">
         <v>276</v>
-      </c>
-      <c r="D122" s="19" t="s">
-        <v>6</v>
-      </c>
-      <c r="H122" s="19" t="s">
-        <v>6</v>
-      </c>
-      <c r="I122" s="32" t="s">
-        <v>277</v>
       </c>
     </row>
     <row r="123" spans="1:9" ht="30" x14ac:dyDescent="0.15">
@@ -4438,7 +4454,7 @@
         <v>131</v>
       </c>
       <c r="B123" s="6" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="E123" s="19" t="s">
         <v>6</v>
@@ -4447,7 +4463,7 @@
         <v>6</v>
       </c>
       <c r="I123" s="32" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="124" spans="1:9" ht="60" x14ac:dyDescent="0.15">
@@ -4455,16 +4471,16 @@
         <v>137</v>
       </c>
       <c r="B124" s="6" t="s">
+        <v>278</v>
+      </c>
+      <c r="D124" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="H124" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="I124" s="32" t="s">
         <v>279</v>
-      </c>
-      <c r="D124" s="19" t="s">
-        <v>6</v>
-      </c>
-      <c r="H124" s="19" t="s">
-        <v>6</v>
-      </c>
-      <c r="I124" s="32" t="s">
-        <v>280</v>
       </c>
     </row>
     <row r="125" spans="1:9" s="27" customFormat="1" ht="15" x14ac:dyDescent="0.15">
@@ -4472,7 +4488,7 @@
         <v>138</v>
       </c>
       <c r="B125" s="27" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="D125" s="26" t="s">
         <v>6</v>
@@ -4484,7 +4500,7 @@
         <v>6</v>
       </c>
       <c r="I125" s="35" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="126" spans="1:9" ht="15" x14ac:dyDescent="0.15">
@@ -4501,7 +4517,7 @@
         <v>6</v>
       </c>
       <c r="I126" s="32" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="127" spans="1:9" ht="15" x14ac:dyDescent="0.15">
@@ -4509,16 +4525,16 @@
         <v>142</v>
       </c>
       <c r="B127" s="6" t="s">
+        <v>282</v>
+      </c>
+      <c r="E127" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="H127" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="I127" s="32" t="s">
         <v>283</v>
-      </c>
-      <c r="E127" s="19" t="s">
-        <v>6</v>
-      </c>
-      <c r="H127" s="19" t="s">
-        <v>6</v>
-      </c>
-      <c r="I127" s="32" t="s">
-        <v>284</v>
       </c>
     </row>
     <row r="128" spans="1:9" s="27" customFormat="1" ht="45" x14ac:dyDescent="0.15">
@@ -4526,7 +4542,7 @@
         <v>141</v>
       </c>
       <c r="B128" s="27" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="D128" s="26" t="s">
         <v>6</v>
@@ -4538,7 +4554,7 @@
         <v>6</v>
       </c>
       <c r="I128" s="35" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="129" spans="1:9" ht="15" x14ac:dyDescent="0.15">
@@ -4555,7 +4571,7 @@
         <v>6</v>
       </c>
       <c r="I129" s="32" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="130" spans="1:9" ht="15" x14ac:dyDescent="0.15">
@@ -4563,7 +4579,7 @@
         <v>144</v>
       </c>
       <c r="B130" s="6" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="E130" s="19" t="s">
         <v>6</v>
@@ -4572,7 +4588,7 @@
         <v>6</v>
       </c>
       <c r="I130" s="32" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="131" spans="1:9" ht="15" x14ac:dyDescent="0.15">
@@ -4589,7 +4605,7 @@
         <v>6</v>
       </c>
       <c r="I131" s="32" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="132" spans="1:9" ht="15" x14ac:dyDescent="0.15">
@@ -4606,7 +4622,7 @@
         <v>6</v>
       </c>
       <c r="I132" s="32" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="133" spans="1:9" ht="15" x14ac:dyDescent="0.15">
@@ -4623,7 +4639,7 @@
         <v>6</v>
       </c>
       <c r="I133" s="32" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="134" spans="1:9" ht="15" x14ac:dyDescent="0.15">
@@ -4631,7 +4647,7 @@
         <v>146</v>
       </c>
       <c r="B134" s="6" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="D134" s="19" t="s">
         <v>6</v>
@@ -4640,7 +4656,7 @@
         <v>6</v>
       </c>
       <c r="I134" s="32" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="135" spans="1:9" ht="135" x14ac:dyDescent="0.15">
@@ -4657,7 +4673,7 @@
         <v>6</v>
       </c>
       <c r="I135" s="32" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="136" spans="1:9" ht="45" x14ac:dyDescent="0.15">
@@ -4665,19 +4681,19 @@
         <v>148</v>
       </c>
       <c r="B136" s="6" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="C136" s="32" t="s">
+        <v>289</v>
+      </c>
+      <c r="D136" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="H136" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="I136" s="32" t="s">
         <v>290</v>
-      </c>
-      <c r="D136" s="19" t="s">
-        <v>6</v>
-      </c>
-      <c r="H136" s="19" t="s">
-        <v>6</v>
-      </c>
-      <c r="I136" s="32" t="s">
-        <v>291</v>
       </c>
     </row>
     <row r="137" spans="1:9" ht="30" x14ac:dyDescent="0.15">
@@ -4685,7 +4701,7 @@
         <v>149</v>
       </c>
       <c r="B137" s="6" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="E137" s="19" t="s">
         <v>6</v>
@@ -4694,7 +4710,7 @@
         <v>6</v>
       </c>
       <c r="I137" s="32" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="138" spans="1:9" ht="75" x14ac:dyDescent="0.15">
@@ -4711,7 +4727,7 @@
         <v>6</v>
       </c>
       <c r="I138" s="32" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="139" spans="1:9" ht="15" x14ac:dyDescent="0.15">
@@ -4728,7 +4744,7 @@
         <v>6</v>
       </c>
       <c r="I139" s="32" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="140" spans="1:9" s="17" customFormat="1" ht="30" x14ac:dyDescent="0.15">
@@ -4736,7 +4752,7 @@
         <v>154</v>
       </c>
       <c r="B140" s="17" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="D140" s="21"/>
       <c r="E140" s="21"/>
@@ -4748,7 +4764,7 @@
         <v>6</v>
       </c>
       <c r="I140" s="33" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="141" spans="1:9" s="17" customFormat="1" ht="15" x14ac:dyDescent="0.15">
@@ -4756,7 +4772,7 @@
         <v>153</v>
       </c>
       <c r="B141" s="17" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="D141" s="21"/>
       <c r="E141" s="21"/>
@@ -4768,7 +4784,7 @@
         <v>6</v>
       </c>
       <c r="I141" s="33" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="142" spans="1:9" s="17" customFormat="1" ht="30" x14ac:dyDescent="0.15">
@@ -4776,7 +4792,7 @@
         <v>155</v>
       </c>
       <c r="B142" s="17" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="D142" s="21"/>
       <c r="E142" s="21"/>
@@ -4788,7 +4804,7 @@
         <v>6</v>
       </c>
       <c r="I142" s="33" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="143" spans="1:9" ht="15" x14ac:dyDescent="0.15">
@@ -4796,7 +4812,7 @@
         <v>152</v>
       </c>
       <c r="B143" s="6" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="D143" s="19" t="s">
         <v>6</v>
@@ -4805,7 +4821,7 @@
         <v>6</v>
       </c>
       <c r="I143" s="32" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="144" spans="1:9" s="27" customFormat="1" ht="60" x14ac:dyDescent="0.15">
@@ -4813,7 +4829,7 @@
         <v>156</v>
       </c>
       <c r="B144" s="27" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D144" s="26" t="s">
         <v>6</v>
@@ -4825,7 +4841,7 @@
         <v>6</v>
       </c>
       <c r="I144" s="35" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="145" spans="1:9" ht="30" x14ac:dyDescent="0.15">
@@ -4842,7 +4858,7 @@
         <v>6</v>
       </c>
       <c r="I145" s="32" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="146" spans="1:9" s="27" customFormat="1" ht="15" x14ac:dyDescent="0.15">
@@ -4850,7 +4866,7 @@
         <v>158</v>
       </c>
       <c r="B146" s="27" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="D146" s="26" t="s">
         <v>6</v>
@@ -4862,7 +4878,7 @@
         <v>6</v>
       </c>
       <c r="I146" s="35" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="147" spans="1:9" ht="15" x14ac:dyDescent="0.15">
@@ -4879,7 +4895,7 @@
         <v>6</v>
       </c>
       <c r="I147" s="32" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="148" spans="1:9" ht="45" x14ac:dyDescent="0.15">
@@ -4887,7 +4903,7 @@
         <v>167</v>
       </c>
       <c r="B148" s="6" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="E148" s="19" t="s">
         <v>6</v>
@@ -4896,7 +4912,7 @@
         <v>6</v>
       </c>
       <c r="I148" s="32" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="149" spans="1:9" s="27" customFormat="1" ht="30" x14ac:dyDescent="0.15">
@@ -4904,7 +4920,7 @@
         <v>165</v>
       </c>
       <c r="B149" s="27" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="D149" s="26"/>
       <c r="E149" s="26" t="s">
@@ -4916,7 +4932,7 @@
         <v>6</v>
       </c>
       <c r="I149" s="35" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="150" spans="1:9" ht="15" x14ac:dyDescent="0.15">
@@ -4933,7 +4949,7 @@
         <v>6</v>
       </c>
       <c r="I150" s="32" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="151" spans="1:9" ht="15" x14ac:dyDescent="0.15">
@@ -4950,7 +4966,7 @@
         <v>6</v>
       </c>
       <c r="I151" s="32" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="152" spans="1:9" ht="30" x14ac:dyDescent="0.15">
@@ -4967,7 +4983,7 @@
         <v>6</v>
       </c>
       <c r="I152" s="32" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="153" spans="1:9" ht="15" x14ac:dyDescent="0.15">
@@ -4984,7 +5000,7 @@
         <v>6</v>
       </c>
       <c r="I153" s="32" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="154" spans="1:9" ht="45" x14ac:dyDescent="0.15">
@@ -5001,7 +5017,7 @@
         <v>6</v>
       </c>
       <c r="I154" s="32" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="155" spans="1:9" ht="15" x14ac:dyDescent="0.15">
@@ -5009,16 +5025,16 @@
         <v>189</v>
       </c>
       <c r="B155" s="6" t="s">
+        <v>307</v>
+      </c>
+      <c r="D155" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="H155" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="I155" s="32" t="s">
         <v>308</v>
-      </c>
-      <c r="D155" s="19" t="s">
-        <v>6</v>
-      </c>
-      <c r="H155" s="19" t="s">
-        <v>6</v>
-      </c>
-      <c r="I155" s="32" t="s">
-        <v>309</v>
       </c>
     </row>
     <row r="156" spans="1:9" s="17" customFormat="1" ht="60" x14ac:dyDescent="0.15">
@@ -5026,7 +5042,7 @@
         <v>193</v>
       </c>
       <c r="B156" s="17" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C156" s="17" t="s">
         <v>35</v>
@@ -5041,7 +5057,7 @@
         <v>6</v>
       </c>
       <c r="I156" s="33" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="157" spans="1:9" ht="15" x14ac:dyDescent="0.15">
@@ -5058,7 +5074,7 @@
         <v>6</v>
       </c>
       <c r="I157" s="32" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="158" spans="1:9" s="27" customFormat="1" ht="30" x14ac:dyDescent="0.15">
@@ -5066,7 +5082,7 @@
         <v>187</v>
       </c>
       <c r="B158" s="27" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="D158" s="26"/>
       <c r="E158" s="26" t="s">
@@ -5078,7 +5094,7 @@
         <v>6</v>
       </c>
       <c r="I158" s="35" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="159" spans="1:9" ht="45" x14ac:dyDescent="0.15">
@@ -5086,7 +5102,7 @@
         <v>186</v>
       </c>
       <c r="B159" s="6" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="D159" s="19" t="s">
         <v>6</v>
@@ -5095,7 +5111,7 @@
         <v>6</v>
       </c>
       <c r="I159" s="32" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="160" spans="1:9" ht="15" x14ac:dyDescent="0.15">
@@ -5103,7 +5119,7 @@
         <v>185</v>
       </c>
       <c r="B160" s="6" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="D160" s="19" t="s">
         <v>6</v>
@@ -5112,7 +5128,7 @@
         <v>6</v>
       </c>
       <c r="I160" s="32" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="161" spans="1:9" ht="15" x14ac:dyDescent="0.15">
@@ -5129,7 +5145,7 @@
         <v>6</v>
       </c>
       <c r="I161" s="32" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="162" spans="1:9" s="27" customFormat="1" ht="30" x14ac:dyDescent="0.15">
@@ -5137,7 +5153,7 @@
         <v>182</v>
       </c>
       <c r="B162" s="27" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="C162" s="35"/>
       <c r="D162" s="26"/>
@@ -5150,7 +5166,7 @@
         <v>6</v>
       </c>
       <c r="I162" s="35" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="163" spans="1:9" ht="15" x14ac:dyDescent="0.15">
@@ -5164,7 +5180,7 @@
         <v>6</v>
       </c>
       <c r="I163" s="32" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="164" spans="1:9" ht="30" x14ac:dyDescent="0.15">
@@ -5178,7 +5194,7 @@
         <v>6</v>
       </c>
       <c r="I164" s="32" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="165" spans="1:9" ht="30" x14ac:dyDescent="0.15">
@@ -5186,13 +5202,13 @@
         <v>179</v>
       </c>
       <c r="B165" s="6" t="s">
+        <v>317</v>
+      </c>
+      <c r="E165" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="I165" s="32" t="s">
         <v>318</v>
-      </c>
-      <c r="E165" s="19" t="s">
-        <v>6</v>
-      </c>
-      <c r="I165" s="32" t="s">
-        <v>319</v>
       </c>
     </row>
     <row r="166" spans="1:9" ht="15" x14ac:dyDescent="0.15">
@@ -5206,7 +5222,7 @@
         <v>6</v>
       </c>
       <c r="I166" s="32" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="167" spans="1:9" s="27" customFormat="1" ht="30" x14ac:dyDescent="0.15">
@@ -5224,7 +5240,7 @@
       <c r="G167" s="47"/>
       <c r="H167" s="26"/>
       <c r="I167" s="35" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="168" spans="1:9" ht="30" x14ac:dyDescent="0.15">
@@ -5238,7 +5254,7 @@
         <v>6</v>
       </c>
       <c r="I168" s="32" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="169" spans="1:9" ht="15" x14ac:dyDescent="0.15">
@@ -5246,13 +5262,13 @@
         <v>174</v>
       </c>
       <c r="B169" s="6" t="s">
+        <v>322</v>
+      </c>
+      <c r="D169" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="I169" s="32" t="s">
         <v>323</v>
-      </c>
-      <c r="D169" s="19" t="s">
-        <v>6</v>
-      </c>
-      <c r="I169" s="32" t="s">
-        <v>324</v>
       </c>
     </row>
     <row r="170" spans="1:9" ht="15" x14ac:dyDescent="0.15">
@@ -5260,13 +5276,13 @@
         <v>173</v>
       </c>
       <c r="B170" s="6" t="s">
+        <v>324</v>
+      </c>
+      <c r="E170" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="I170" s="32" t="s">
         <v>325</v>
-      </c>
-      <c r="E170" s="19" t="s">
-        <v>6</v>
-      </c>
-      <c r="I170" s="32" t="s">
-        <v>326</v>
       </c>
     </row>
     <row r="171" spans="1:9" ht="30" x14ac:dyDescent="0.15">
@@ -5280,15 +5296,15 @@
         <v>6</v>
       </c>
       <c r="I171" s="32" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="172" spans="1:9" s="17" customFormat="1" ht="30" x14ac:dyDescent="0.15">
       <c r="A172" s="17" t="s">
+        <v>327</v>
+      </c>
+      <c r="B172" s="17" t="s">
         <v>328</v>
-      </c>
-      <c r="B172" s="17" t="s">
-        <v>329</v>
       </c>
       <c r="D172" s="21"/>
       <c r="E172" s="21"/>
@@ -5298,12 +5314,12 @@
       <c r="G172" s="48"/>
       <c r="H172" s="21"/>
       <c r="I172" s="33" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
     </row>
     <row r="173" spans="1:9" ht="15" x14ac:dyDescent="0.15">
       <c r="A173" s="6" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="B173" s="6" t="s">
         <v>168</v>
@@ -5312,18 +5328,18 @@
         <v>6</v>
       </c>
       <c r="I173" s="32" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="174" spans="1:9" s="17" customFormat="1" ht="60" x14ac:dyDescent="0.15">
       <c r="A174" s="17" t="s">
+        <v>332</v>
+      </c>
+      <c r="B174" s="17" t="s">
         <v>333</v>
       </c>
-      <c r="B174" s="17" t="s">
-        <v>334</v>
-      </c>
       <c r="C174" s="17" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="D174" s="21"/>
       <c r="E174" s="21"/>
@@ -5333,12 +5349,12 @@
       <c r="G174" s="48"/>
       <c r="H174" s="21"/>
       <c r="I174" s="33" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="175" spans="1:9" ht="15" x14ac:dyDescent="0.15">
       <c r="A175" s="6" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="B175" s="6" t="s">
         <v>74</v>
@@ -5347,12 +5363,12 @@
         <v>6</v>
       </c>
       <c r="I175" s="32" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="176" spans="1:9" ht="15" x14ac:dyDescent="0.15">
       <c r="A176" s="6" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="B176" s="6" t="s">
         <v>116</v>
@@ -5361,12 +5377,12 @@
         <v>6</v>
       </c>
       <c r="I176" s="32" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="177" spans="1:9" s="27" customFormat="1" ht="15" x14ac:dyDescent="0.15">
       <c r="A177" s="27" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="B177" s="27" t="s">
         <v>28</v>
@@ -5379,15 +5395,15 @@
       <c r="G177" s="47"/>
       <c r="H177" s="26"/>
       <c r="I177" s="35" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
     <row r="178" spans="1:9" s="17" customFormat="1" ht="30" x14ac:dyDescent="0.15">
       <c r="A178" s="17" t="s">
+        <v>341</v>
+      </c>
+      <c r="B178" s="17" t="s">
         <v>342</v>
-      </c>
-      <c r="B178" s="17" t="s">
-        <v>343</v>
       </c>
       <c r="D178" s="21"/>
       <c r="E178" s="21" t="s">
@@ -5397,26 +5413,26 @@
       <c r="G178" s="48"/>
       <c r="H178" s="21"/>
       <c r="I178" s="33" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="179" spans="1:9" ht="30" x14ac:dyDescent="0.15">
       <c r="A179" s="6" t="s">
+        <v>344</v>
+      </c>
+      <c r="B179" s="6" t="s">
         <v>345</v>
       </c>
-      <c r="B179" s="6" t="s">
+      <c r="E179" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="I179" s="32" t="s">
         <v>346</v>
-      </c>
-      <c r="E179" s="19" t="s">
-        <v>6</v>
-      </c>
-      <c r="I179" s="32" t="s">
-        <v>347</v>
       </c>
     </row>
     <row r="180" spans="1:9" s="27" customFormat="1" ht="60" x14ac:dyDescent="0.15">
       <c r="A180" s="27" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B180" s="27" t="s">
         <v>15</v>
@@ -5429,15 +5445,15 @@
       <c r="G180" s="47"/>
       <c r="H180" s="26"/>
       <c r="I180" s="35" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="181" spans="1:9" s="17" customFormat="1" ht="45" x14ac:dyDescent="0.15">
       <c r="A181" s="17" t="s">
+        <v>349</v>
+      </c>
+      <c r="B181" s="17" t="s">
         <v>350</v>
-      </c>
-      <c r="B181" s="17" t="s">
-        <v>351</v>
       </c>
       <c r="D181" s="21"/>
       <c r="E181" s="21"/>
@@ -5447,12 +5463,12 @@
       <c r="G181" s="48"/>
       <c r="H181" s="21"/>
       <c r="I181" s="33" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
     </row>
     <row r="182" spans="1:9" ht="30" x14ac:dyDescent="0.15">
       <c r="A182" s="6" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="B182" s="6" t="s">
         <v>15</v>
@@ -5461,26 +5477,26 @@
         <v>6</v>
       </c>
       <c r="I182" s="32" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="183" spans="1:9" ht="15" x14ac:dyDescent="0.15">
       <c r="A183" s="6" t="s">
+        <v>354</v>
+      </c>
+      <c r="B183" s="6" t="s">
         <v>355</v>
       </c>
-      <c r="B183" s="6" t="s">
+      <c r="E183" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="I183" s="32" t="s">
         <v>356</v>
-      </c>
-      <c r="E183" s="19" t="s">
-        <v>6</v>
-      </c>
-      <c r="I183" s="32" t="s">
-        <v>357</v>
       </c>
     </row>
     <row r="184" spans="1:9" ht="15" x14ac:dyDescent="0.15">
       <c r="A184" s="6" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="B184" s="6" t="s">
         <v>76</v>
@@ -5489,21 +5505,21 @@
         <v>6</v>
       </c>
       <c r="I184" s="32" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="185" spans="1:9" ht="90" x14ac:dyDescent="0.15">
       <c r="A185" s="6" t="s">
+        <v>359</v>
+      </c>
+      <c r="B185" s="6" t="s">
         <v>360</v>
       </c>
-      <c r="B185" s="6" t="s">
+      <c r="F185" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="I185" s="32" t="s">
         <v>361</v>
-      </c>
-      <c r="F185" s="19" t="s">
-        <v>6</v>
-      </c>
-      <c r="I185" s="32" t="s">
-        <v>362</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Feb 7 2024 Update
</commit_message>
<xml_diff>
--- a/SQL/leetcode - sql.xlsx
+++ b/SQL/leetcode - sql.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zw/Documents/Github/LeetCode_Practice/SQL/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71183AB9-6593-5B46-B63E-83B93810ED5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4524733-3EB4-7C49-86C3-45ED4A183E26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="950" uniqueCount="462">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="962" uniqueCount="463">
   <si>
     <t>Title</t>
   </si>
@@ -714,9 +714,6 @@
   </si>
   <si>
     <t>这种简单的题不要用cte，因为简单所以面试的时候需要直接写出来</t>
-  </si>
-  <si>
-    <t>这种题可以用rank也可以直接用最基础的，先找出最大值，然后再原表中找到等于最大值的</t>
   </si>
   <si>
     <t>易错题。我是因为做了很多次所以在这道题上留了个心眼。但是坑还是这道题坑，因为我们要找买了A没买B的buyer，那么我们的where定位是不能用product定位的，而只能用buyer去做定位</t>
@@ -1602,6 +1599,14 @@
     <t>想通了其实就很简单，只需要保证两点：
 1. Customer的product是在Product表里面的 
 2.从Customer表中计算的product数量和从Product表中抽出来的数量一致</t>
+  </si>
+  <si>
+    <t>这种题可以用rank也可以直接用最基础的，先找出最大值，然后再原表中找到等于最大值的。
+排序问题是可以求和排序的，但是这种情况就和一般求和一样需要group by</t>
+  </si>
+  <si>
+    <t>1083. Sales Analysis II
+1084. Sales Analysis III</t>
   </si>
 </sst>
 </file>
@@ -2106,8 +2111,8 @@
   <dimension ref="A1:I185"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="112" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A48" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A56" sqref="A56:XFD56"/>
+      <pane ySplit="6" topLeftCell="A61" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F66" sqref="F66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="28" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -2171,10 +2176,10 @@
         <v>1</v>
       </c>
       <c r="G6" s="45" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="H6" s="12" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="I6" s="11" t="s">
         <v>194</v>
@@ -2221,7 +2226,7 @@
         <v>6</v>
       </c>
       <c r="I8" s="4" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="9" spans="1:9" s="27" customFormat="1" ht="76" thickBot="1" x14ac:dyDescent="0.2">
@@ -2244,7 +2249,7 @@
         <v>6</v>
       </c>
       <c r="I9" s="25" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="91" thickBot="1" x14ac:dyDescent="0.2">
@@ -2265,7 +2270,7 @@
         <v>6</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
     </row>
     <row r="11" spans="1:9" s="14" customFormat="1" ht="61" thickBot="1" x14ac:dyDescent="0.2">
@@ -2288,7 +2293,7 @@
         <v>6</v>
       </c>
       <c r="I11" s="4" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.2">
@@ -2338,7 +2343,7 @@
         <v>21</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C14" s="2"/>
       <c r="D14" s="19" t="s">
@@ -2351,7 +2356,7 @@
         <v>6</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="31" thickBot="1" x14ac:dyDescent="0.2">
@@ -2372,7 +2377,7 @@
         <v>6</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="31" thickBot="1" x14ac:dyDescent="0.2">
@@ -2418,7 +2423,7 @@
         <v>6</v>
       </c>
       <c r="I17" s="25" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
     </row>
     <row r="18" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.2">
@@ -2449,7 +2454,7 @@
         <v>29</v>
       </c>
       <c r="B19" s="16" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="C19" s="16"/>
       <c r="D19" s="21"/>
@@ -2464,7 +2469,7 @@
         <v>6</v>
       </c>
       <c r="I19" s="29" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
     </row>
     <row r="20" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.2">
@@ -2493,7 +2498,7 @@
         <v>31</v>
       </c>
       <c r="B21" s="41" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="C21" s="2"/>
       <c r="D21" s="19" t="s">
@@ -2506,7 +2511,7 @@
         <v>6</v>
       </c>
       <c r="I21" s="40" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="22" spans="1:9" s="27" customFormat="1" ht="46" thickBot="1" x14ac:dyDescent="0.2">
@@ -2514,7 +2519,7 @@
         <v>32</v>
       </c>
       <c r="B22" s="50" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="C22" s="25"/>
       <c r="D22" s="26"/>
@@ -2529,7 +2534,7 @@
         <v>6</v>
       </c>
       <c r="I22" s="51" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
     </row>
     <row r="23" spans="1:9" ht="31" thickBot="1" x14ac:dyDescent="0.2">
@@ -2550,7 +2555,7 @@
         <v>6</v>
       </c>
       <c r="I23" s="40" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
     </row>
     <row r="24" spans="1:9" s="17" customFormat="1" ht="91" thickBot="1" x14ac:dyDescent="0.2">
@@ -2575,7 +2580,7 @@
         <v>6</v>
       </c>
       <c r="I24" s="29" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
     </row>
     <row r="25" spans="1:9" s="14" customFormat="1" ht="46" thickBot="1" x14ac:dyDescent="0.2">
@@ -2598,7 +2603,7 @@
         <v>6</v>
       </c>
       <c r="I25" s="53" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="26" spans="1:9" s="17" customFormat="1" ht="409.6" thickBot="1" x14ac:dyDescent="0.2">
@@ -2606,7 +2611,7 @@
         <v>35</v>
       </c>
       <c r="B26" s="16" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="C26" s="28" t="s">
         <v>34</v>
@@ -2623,7 +2628,7 @@
         <v>6</v>
       </c>
       <c r="I26" s="29" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
     </row>
     <row r="27" spans="1:9" ht="31" thickBot="1" x14ac:dyDescent="0.2">
@@ -2631,7 +2636,7 @@
         <v>37</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="C27" s="2"/>
       <c r="E27" s="19" t="s">
@@ -2644,7 +2649,7 @@
         <v>6</v>
       </c>
       <c r="I27" s="24" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
     <row r="28" spans="1:9" ht="46" thickBot="1" x14ac:dyDescent="0.2">
@@ -2652,7 +2657,7 @@
         <v>8</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="C28" s="1"/>
       <c r="D28" s="19" t="s">
@@ -2665,7 +2670,7 @@
         <v>6</v>
       </c>
       <c r="I28" s="32" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="29" spans="1:9" ht="210" x14ac:dyDescent="0.15">
@@ -2685,7 +2690,7 @@
         <v>6</v>
       </c>
       <c r="I29" s="32" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="30" spans="1:9" s="17" customFormat="1" ht="255" x14ac:dyDescent="0.15">
@@ -2693,7 +2698,7 @@
         <v>40</v>
       </c>
       <c r="B30" s="17" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="D30" s="21"/>
       <c r="E30" s="21"/>
@@ -2747,7 +2752,7 @@
         <v>6</v>
       </c>
       <c r="I32" s="32" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="33" spans="1:9" ht="46" thickBot="1" x14ac:dyDescent="0.2">
@@ -2767,7 +2772,7 @@
         <v>6</v>
       </c>
       <c r="I33" s="32" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="34" spans="1:9" ht="15" x14ac:dyDescent="0.15">
@@ -2849,7 +2854,7 @@
         <v>6</v>
       </c>
       <c r="I37" s="35" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
     <row r="38" spans="1:9" s="17" customFormat="1" ht="180" x14ac:dyDescent="0.15">
@@ -2874,7 +2879,7 @@
         <v>6</v>
       </c>
       <c r="I38" s="33" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
     </row>
     <row r="39" spans="1:9" ht="30" x14ac:dyDescent="0.15">
@@ -2882,7 +2887,7 @@
         <v>50</v>
       </c>
       <c r="B39" s="6" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="E39" s="19" t="s">
         <v>6</v>
@@ -2917,7 +2922,7 @@
         <v>6</v>
       </c>
       <c r="I40" s="32" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="41" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.2">
@@ -2925,7 +2930,7 @@
         <v>51</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="D41" s="19" t="s">
         <v>6</v>
@@ -2937,7 +2942,7 @@
         <v>6</v>
       </c>
       <c r="I41" s="32" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
     </row>
     <row r="42" spans="1:9" ht="30" x14ac:dyDescent="0.15">
@@ -2945,7 +2950,7 @@
         <v>52</v>
       </c>
       <c r="B42" s="6" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="E42" s="19" t="s">
         <v>6</v>
@@ -2957,7 +2962,7 @@
         <v>6</v>
       </c>
       <c r="I42" s="32" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
     </row>
     <row r="43" spans="1:9" ht="30" x14ac:dyDescent="0.15">
@@ -2965,7 +2970,7 @@
         <v>53</v>
       </c>
       <c r="B43" s="6" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="D43" s="19" t="s">
         <v>6</v>
@@ -2985,7 +2990,7 @@
         <v>160</v>
       </c>
       <c r="B44" s="27" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="C44" s="27" t="s">
         <v>161</v>
@@ -3002,7 +3007,7 @@
         <v>6</v>
       </c>
       <c r="I44" s="35" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
     </row>
     <row r="45" spans="1:9" ht="15" x14ac:dyDescent="0.15">
@@ -3053,7 +3058,7 @@
         <v>132</v>
       </c>
       <c r="B47" s="6" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="C47" s="6" t="s">
         <v>73</v>
@@ -3068,7 +3073,7 @@
         <v>6</v>
       </c>
       <c r="I47" s="32" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
     </row>
     <row r="48" spans="1:9" s="17" customFormat="1" ht="75" x14ac:dyDescent="0.15">
@@ -3090,7 +3095,7 @@
         <v>6</v>
       </c>
       <c r="I48" s="33" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
     </row>
     <row r="49" spans="1:9" s="14" customFormat="1" ht="30" x14ac:dyDescent="0.15">
@@ -3132,7 +3137,7 @@
         <v>6</v>
       </c>
       <c r="I50" s="32" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
     </row>
     <row r="51" spans="1:9" s="17" customFormat="1" ht="60" x14ac:dyDescent="0.15">
@@ -3154,7 +3159,7 @@
         <v>6</v>
       </c>
       <c r="I51" s="33" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
     </row>
     <row r="52" spans="1:9" s="27" customFormat="1" ht="15" x14ac:dyDescent="0.15">
@@ -3162,7 +3167,7 @@
         <v>55</v>
       </c>
       <c r="B52" s="27" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="D52" s="26" t="s">
         <v>6</v>
@@ -3196,7 +3201,7 @@
         <v>6</v>
       </c>
       <c r="I53" s="32" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
     </row>
     <row r="54" spans="1:9" ht="15" x14ac:dyDescent="0.15">
@@ -3264,16 +3269,19 @@
         <v>61</v>
       </c>
       <c r="B57" s="6" t="s">
+        <v>392</v>
+      </c>
+      <c r="E57" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="G57" s="44" t="s">
+        <v>6</v>
+      </c>
+      <c r="H57" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="I57" s="32" t="s">
         <v>393</v>
-      </c>
-      <c r="E57" s="19" t="s">
-        <v>6</v>
-      </c>
-      <c r="H57" s="19" t="s">
-        <v>6</v>
-      </c>
-      <c r="I57" s="32" t="s">
-        <v>394</v>
       </c>
     </row>
     <row r="58" spans="1:9" ht="15" x14ac:dyDescent="0.15">
@@ -3286,6 +3294,9 @@
       <c r="D58" s="19" t="s">
         <v>6</v>
       </c>
+      <c r="G58" s="44" t="s">
+        <v>6</v>
+      </c>
       <c r="H58" s="19" t="s">
         <v>6</v>
       </c>
@@ -3293,7 +3304,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="59" spans="1:9" ht="30" x14ac:dyDescent="0.15">
+    <row r="59" spans="1:9" ht="60" x14ac:dyDescent="0.15">
       <c r="A59" s="6" t="s">
         <v>63</v>
       </c>
@@ -3306,11 +3317,14 @@
       <c r="D59" s="19" t="s">
         <v>6</v>
       </c>
+      <c r="G59" s="44" t="s">
+        <v>6</v>
+      </c>
       <c r="H59" s="19" t="s">
         <v>6</v>
       </c>
       <c r="I59" s="32" t="s">
-        <v>225</v>
+        <v>461</v>
       </c>
     </row>
     <row r="60" spans="1:9" ht="45" x14ac:dyDescent="0.15">
@@ -3323,11 +3337,14 @@
       <c r="E60" s="19" t="s">
         <v>6</v>
       </c>
+      <c r="G60" s="44" t="s">
+        <v>6</v>
+      </c>
       <c r="H60" s="19" t="s">
         <v>6</v>
       </c>
       <c r="I60" s="32" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
     <row r="61" spans="1:9" ht="15" x14ac:dyDescent="0.15">
@@ -3343,11 +3360,14 @@
       <c r="D61" s="19" t="s">
         <v>6</v>
       </c>
+      <c r="G61" s="44" t="s">
+        <v>6</v>
+      </c>
       <c r="H61" s="19" t="s">
         <v>6</v>
       </c>
       <c r="I61" s="32" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
     </row>
     <row r="62" spans="1:9" s="14" customFormat="1" ht="45" x14ac:dyDescent="0.15">
@@ -3355,36 +3375,43 @@
         <v>66</v>
       </c>
       <c r="B62" s="14" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="D62" s="20" t="s">
         <v>6</v>
       </c>
       <c r="E62" s="20"/>
       <c r="F62" s="20"/>
-      <c r="G62" s="46"/>
+      <c r="G62" s="46" t="s">
+        <v>6</v>
+      </c>
       <c r="H62" s="20" t="s">
         <v>6</v>
       </c>
       <c r="I62" s="34" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="63" spans="1:9" ht="46" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A63" s="6" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" s="14" customFormat="1" ht="46" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A63" s="14" t="s">
         <v>67</v>
       </c>
-      <c r="B63" s="6" t="s">
-        <v>228</v>
-      </c>
-      <c r="D63" s="19" t="s">
-        <v>6</v>
-      </c>
-      <c r="H63" s="19" t="s">
-        <v>6</v>
-      </c>
-      <c r="I63" s="32" t="s">
-        <v>397</v>
+      <c r="B63" s="14" t="s">
+        <v>227</v>
+      </c>
+      <c r="D63" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="E63" s="20"/>
+      <c r="F63" s="20"/>
+      <c r="G63" s="46" t="s">
+        <v>6</v>
+      </c>
+      <c r="H63" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="I63" s="34" t="s">
+        <v>396</v>
       </c>
     </row>
     <row r="64" spans="1:9" ht="31" thickBot="1" x14ac:dyDescent="0.2">
@@ -3392,17 +3419,20 @@
         <v>68</v>
       </c>
       <c r="B64" s="41" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="C64" s="2"/>
       <c r="F64" s="19" t="s">
         <v>6</v>
       </c>
+      <c r="G64" s="44" t="s">
+        <v>6</v>
+      </c>
       <c r="H64" s="19" t="s">
         <v>6</v>
       </c>
       <c r="I64" s="40" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="65" spans="1:9" s="14" customFormat="1" ht="105" x14ac:dyDescent="0.15">
@@ -3410,19 +3440,24 @@
         <v>69</v>
       </c>
       <c r="B65" s="14" t="s">
-        <v>230</v>
+        <v>229</v>
+      </c>
+      <c r="C65" s="34" t="s">
+        <v>462</v>
       </c>
       <c r="D65" s="20"/>
       <c r="E65" s="20" t="s">
         <v>6</v>
       </c>
       <c r="F65" s="20"/>
-      <c r="G65" s="46"/>
+      <c r="G65" s="46" t="s">
+        <v>6</v>
+      </c>
       <c r="H65" s="20" t="s">
         <v>6</v>
       </c>
       <c r="I65" s="34" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
     </row>
     <row r="66" spans="1:9" ht="15" x14ac:dyDescent="0.15">
@@ -3430,16 +3465,19 @@
         <v>70</v>
       </c>
       <c r="B66" s="6" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="E66" s="19" t="s">
         <v>6</v>
       </c>
+      <c r="G66" s="44" t="s">
+        <v>6</v>
+      </c>
       <c r="H66" s="19" t="s">
         <v>6</v>
       </c>
       <c r="I66" s="32" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="67" spans="1:9" ht="15" x14ac:dyDescent="0.15">
@@ -3452,11 +3490,14 @@
       <c r="E67" s="19" t="s">
         <v>6</v>
       </c>
+      <c r="G67" s="44" t="s">
+        <v>6</v>
+      </c>
       <c r="H67" s="19" t="s">
         <v>6</v>
       </c>
       <c r="I67" s="32" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="68" spans="1:9" ht="15" x14ac:dyDescent="0.15">
@@ -3473,7 +3514,7 @@
         <v>6</v>
       </c>
       <c r="I68" s="32" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="69" spans="1:9" ht="30" x14ac:dyDescent="0.15">
@@ -3493,7 +3534,7 @@
         <v>6</v>
       </c>
       <c r="I69" s="32" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="70" spans="1:9" s="17" customFormat="1" ht="90" x14ac:dyDescent="0.15">
@@ -3501,7 +3542,7 @@
         <v>75</v>
       </c>
       <c r="B70" s="17" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D70" s="21"/>
       <c r="E70" s="21"/>
@@ -3513,7 +3554,7 @@
         <v>6</v>
       </c>
       <c r="I70" s="33" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.15">
@@ -3530,7 +3571,7 @@
         <v>6</v>
       </c>
       <c r="I71" s="6" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="72" spans="1:9" ht="30" x14ac:dyDescent="0.15">
@@ -3547,7 +3588,7 @@
         <v>6</v>
       </c>
       <c r="I72" s="32" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="73" spans="1:9" ht="30" x14ac:dyDescent="0.15">
@@ -3564,7 +3605,7 @@
         <v>6</v>
       </c>
       <c r="I73" s="32" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="74" spans="1:9" ht="15" x14ac:dyDescent="0.15">
@@ -3581,7 +3622,7 @@
         <v>6</v>
       </c>
       <c r="I74" s="32" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="75" spans="1:9" s="14" customFormat="1" ht="75" x14ac:dyDescent="0.15">
@@ -3601,7 +3642,7 @@
         <v>6</v>
       </c>
       <c r="I75" s="34" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
     </row>
     <row r="76" spans="1:9" ht="60" x14ac:dyDescent="0.15">
@@ -3618,7 +3659,7 @@
         <v>6</v>
       </c>
       <c r="I76" s="32" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
     </row>
     <row r="77" spans="1:9" ht="30" x14ac:dyDescent="0.15">
@@ -3626,7 +3667,7 @@
         <v>85</v>
       </c>
       <c r="B77" s="6" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="F77" s="19" t="s">
         <v>6</v>
@@ -3635,7 +3676,7 @@
         <v>6</v>
       </c>
       <c r="I77" s="32" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="78" spans="1:9" ht="30" x14ac:dyDescent="0.15">
@@ -3643,7 +3684,7 @@
         <v>86</v>
       </c>
       <c r="B78" s="6" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="E78" s="19" t="s">
         <v>6</v>
@@ -3652,7 +3693,7 @@
         <v>6</v>
       </c>
       <c r="I78" s="32" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="79" spans="1:9" ht="15" x14ac:dyDescent="0.15">
@@ -3660,7 +3701,7 @@
         <v>87</v>
       </c>
       <c r="B79" s="6" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="D79" s="19" t="s">
         <v>6</v>
@@ -3669,7 +3710,7 @@
         <v>6</v>
       </c>
       <c r="I79" s="32" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="80" spans="1:9" ht="45" x14ac:dyDescent="0.15">
@@ -3677,7 +3718,7 @@
         <v>88</v>
       </c>
       <c r="B80" s="6" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="E80" s="19" t="s">
         <v>6</v>
@@ -3686,7 +3727,7 @@
         <v>6</v>
       </c>
       <c r="I80" s="32" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
     </row>
     <row r="81" spans="1:9" ht="30" x14ac:dyDescent="0.15">
@@ -3694,7 +3735,7 @@
         <v>89</v>
       </c>
       <c r="B81" s="6" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="D81" s="19" t="s">
         <v>6</v>
@@ -3703,7 +3744,7 @@
         <v>6</v>
       </c>
       <c r="I81" s="32" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="82" spans="1:9" ht="15" x14ac:dyDescent="0.15">
@@ -3711,7 +3752,7 @@
         <v>90</v>
       </c>
       <c r="B82" s="6" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="E82" s="19" t="s">
         <v>6</v>
@@ -3720,7 +3761,7 @@
         <v>6</v>
       </c>
       <c r="I82" s="32" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="83" spans="1:9" ht="45" x14ac:dyDescent="0.15">
@@ -3728,7 +3769,7 @@
         <v>91</v>
       </c>
       <c r="B83" s="6" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="F83" s="19" t="s">
         <v>6</v>
@@ -3737,7 +3778,7 @@
         <v>6</v>
       </c>
       <c r="I83" s="32" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="84" spans="1:9" ht="15" x14ac:dyDescent="0.15">
@@ -3745,7 +3786,7 @@
         <v>92</v>
       </c>
       <c r="B84" s="6" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="E84" s="19" t="s">
         <v>6</v>
@@ -3754,7 +3795,7 @@
         <v>6</v>
       </c>
       <c r="I84" s="32" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="85" spans="1:9" s="17" customFormat="1" ht="45" x14ac:dyDescent="0.15">
@@ -3762,7 +3803,7 @@
         <v>93</v>
       </c>
       <c r="B85" s="17" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="D85" s="21"/>
       <c r="E85" s="21" t="s">
@@ -3774,7 +3815,7 @@
         <v>6</v>
       </c>
       <c r="I85" s="33" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="86" spans="1:9" ht="15" x14ac:dyDescent="0.15">
@@ -3782,7 +3823,7 @@
         <v>94</v>
       </c>
       <c r="B86" s="6" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="D86" s="19" t="s">
         <v>6</v>
@@ -3791,7 +3832,7 @@
         <v>6</v>
       </c>
       <c r="I86" s="32" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="87" spans="1:9" ht="15" x14ac:dyDescent="0.15">
@@ -3799,7 +3840,7 @@
         <v>95</v>
       </c>
       <c r="B87" s="6" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="E87" s="19" t="s">
         <v>6</v>
@@ -3808,7 +3849,7 @@
         <v>6</v>
       </c>
       <c r="I87" s="32" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="88" spans="1:9" s="17" customFormat="1" ht="150" x14ac:dyDescent="0.15">
@@ -3816,7 +3857,7 @@
         <v>98</v>
       </c>
       <c r="B88" s="17" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="C88" s="33"/>
       <c r="D88" s="21"/>
@@ -3829,7 +3870,7 @@
         <v>6</v>
       </c>
       <c r="I88" s="33" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
     </row>
     <row r="89" spans="1:9" ht="15" x14ac:dyDescent="0.15">
@@ -3846,7 +3887,7 @@
         <v>6</v>
       </c>
       <c r="I89" s="32" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="90" spans="1:9" ht="15" x14ac:dyDescent="0.15">
@@ -3863,7 +3904,7 @@
         <v>6</v>
       </c>
       <c r="I90" s="32" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="91" spans="1:9" ht="15" x14ac:dyDescent="0.15">
@@ -3871,7 +3912,7 @@
         <v>99</v>
       </c>
       <c r="B91" s="6" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="E91" s="19" t="s">
         <v>6</v>
@@ -3880,7 +3921,7 @@
         <v>6</v>
       </c>
       <c r="I91" s="32" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="92" spans="1:9" ht="15" x14ac:dyDescent="0.15">
@@ -3888,7 +3929,7 @@
         <v>100</v>
       </c>
       <c r="B92" s="6" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="E92" s="19" t="s">
         <v>6</v>
@@ -3897,7 +3938,7 @@
         <v>6</v>
       </c>
       <c r="I92" s="32" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="93" spans="1:9" s="14" customFormat="1" ht="75" x14ac:dyDescent="0.15">
@@ -3917,7 +3958,7 @@
         <v>6</v>
       </c>
       <c r="I93" s="34" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="94" spans="1:9" ht="15" x14ac:dyDescent="0.15">
@@ -3937,7 +3978,7 @@
         <v>6</v>
       </c>
       <c r="I94" s="32" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="95" spans="1:9" ht="30" x14ac:dyDescent="0.15">
@@ -3945,7 +3986,7 @@
         <v>103</v>
       </c>
       <c r="B95" s="6" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="D95" s="19" t="s">
         <v>6</v>
@@ -3954,7 +3995,7 @@
         <v>6</v>
       </c>
       <c r="I95" s="32" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
     </row>
     <row r="96" spans="1:9" s="27" customFormat="1" ht="60" x14ac:dyDescent="0.15">
@@ -3962,7 +4003,7 @@
         <v>104</v>
       </c>
       <c r="B96" s="27" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="D96" s="26" t="s">
         <v>6</v>
@@ -3974,7 +4015,7 @@
         <v>6</v>
       </c>
       <c r="I96" s="35" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
     </row>
     <row r="97" spans="1:9" ht="15" x14ac:dyDescent="0.15">
@@ -3982,7 +4023,7 @@
         <v>105</v>
       </c>
       <c r="B97" s="6" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="E97" s="19" t="s">
         <v>6</v>
@@ -3991,7 +4032,7 @@
         <v>6</v>
       </c>
       <c r="I97" s="32" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="98" spans="1:9" s="27" customFormat="1" ht="45" x14ac:dyDescent="0.15">
@@ -3999,7 +4040,7 @@
         <v>106</v>
       </c>
       <c r="B98" s="27" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D98" s="26"/>
       <c r="E98" s="26" t="s">
@@ -4011,7 +4052,7 @@
         <v>6</v>
       </c>
       <c r="I98" s="35" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="99" spans="1:9" ht="45" x14ac:dyDescent="0.15">
@@ -4019,7 +4060,7 @@
         <v>107</v>
       </c>
       <c r="B99" s="6" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="D99" s="19" t="s">
         <v>6</v>
@@ -4028,7 +4069,7 @@
         <v>6</v>
       </c>
       <c r="I99" s="32" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="100" spans="1:9" ht="15" x14ac:dyDescent="0.15">
@@ -4045,7 +4086,7 @@
         <v>6</v>
       </c>
       <c r="I100" s="32" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="101" spans="1:9" s="17" customFormat="1" ht="180" x14ac:dyDescent="0.15">
@@ -4053,7 +4094,7 @@
         <v>112</v>
       </c>
       <c r="B101" s="17" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="D101" s="21"/>
       <c r="E101" s="21"/>
@@ -4065,7 +4106,7 @@
         <v>6</v>
       </c>
       <c r="I101" s="33" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="102" spans="1:9" ht="15" x14ac:dyDescent="0.15">
@@ -4082,7 +4123,7 @@
         <v>6</v>
       </c>
       <c r="I102" s="32" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="103" spans="1:9" ht="15" x14ac:dyDescent="0.15">
@@ -4090,7 +4131,7 @@
         <v>110</v>
       </c>
       <c r="B103" s="6" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="D103" s="19" t="s">
         <v>6</v>
@@ -4099,7 +4140,7 @@
         <v>6</v>
       </c>
       <c r="I103" s="32" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="104" spans="1:9" ht="60" x14ac:dyDescent="0.15">
@@ -4107,7 +4148,7 @@
         <v>113</v>
       </c>
       <c r="B104" s="6" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="E104" s="19" t="s">
         <v>6</v>
@@ -4116,7 +4157,7 @@
         <v>6</v>
       </c>
       <c r="I104" s="32" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="105" spans="1:9" ht="45" x14ac:dyDescent="0.15">
@@ -4124,16 +4165,16 @@
         <v>115</v>
       </c>
       <c r="B105" s="6" t="s">
+        <v>424</v>
+      </c>
+      <c r="E105" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="H105" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="I105" s="32" t="s">
         <v>425</v>
-      </c>
-      <c r="E105" s="19" t="s">
-        <v>6</v>
-      </c>
-      <c r="H105" s="19" t="s">
-        <v>6</v>
-      </c>
-      <c r="I105" s="32" t="s">
-        <v>426</v>
       </c>
     </row>
     <row r="106" spans="1:9" s="27" customFormat="1" ht="90" x14ac:dyDescent="0.15">
@@ -4141,7 +4182,7 @@
         <v>118</v>
       </c>
       <c r="B106" s="27" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="D106" s="26"/>
       <c r="E106" s="26"/>
@@ -4153,7 +4194,7 @@
         <v>6</v>
       </c>
       <c r="I106" s="35" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="107" spans="1:9" ht="15" x14ac:dyDescent="0.15">
@@ -4170,7 +4211,7 @@
         <v>6</v>
       </c>
       <c r="I107" s="32" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="108" spans="1:9" s="17" customFormat="1" ht="45" x14ac:dyDescent="0.15">
@@ -4178,7 +4219,7 @@
         <v>119</v>
       </c>
       <c r="B108" s="17" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="D108" s="21"/>
       <c r="E108" s="21"/>
@@ -4190,7 +4231,7 @@
         <v>6</v>
       </c>
       <c r="I108" s="33" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="109" spans="1:9" ht="15" x14ac:dyDescent="0.15">
@@ -4198,7 +4239,7 @@
         <v>120</v>
       </c>
       <c r="B109" s="6" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="E109" s="19" t="s">
         <v>6</v>
@@ -4207,7 +4248,7 @@
         <v>6</v>
       </c>
       <c r="I109" s="32" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="110" spans="1:9" ht="60" x14ac:dyDescent="0.15">
@@ -4224,7 +4265,7 @@
         <v>6</v>
       </c>
       <c r="I110" s="32" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="111" spans="1:9" ht="15" x14ac:dyDescent="0.15">
@@ -4241,7 +4282,7 @@
         <v>6</v>
       </c>
       <c r="I111" s="32" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="112" spans="1:9" s="14" customFormat="1" ht="46" x14ac:dyDescent="0.2">
@@ -4249,7 +4290,7 @@
         <v>124</v>
       </c>
       <c r="B112" s="42" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C112" s="14" t="s">
         <v>121</v>
@@ -4264,7 +4305,7 @@
         <v>6</v>
       </c>
       <c r="I112" s="34" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="113" spans="1:9" ht="15" x14ac:dyDescent="0.15">
@@ -4281,7 +4322,7 @@
         <v>6</v>
       </c>
       <c r="I113" s="32" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="114" spans="1:9" ht="30" x14ac:dyDescent="0.15">
@@ -4289,7 +4330,7 @@
         <v>125</v>
       </c>
       <c r="B114" s="6" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="D114" s="19" t="s">
         <v>6</v>
@@ -4298,7 +4339,7 @@
         <v>6</v>
       </c>
       <c r="I114" s="32" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="115" spans="1:9" s="17" customFormat="1" ht="30" x14ac:dyDescent="0.15">
@@ -4306,7 +4347,7 @@
         <v>126</v>
       </c>
       <c r="B115" s="17" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="D115" s="21"/>
       <c r="E115" s="21" t="s">
@@ -4318,7 +4359,7 @@
         <v>6</v>
       </c>
       <c r="I115" s="33" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="116" spans="1:9" ht="15" x14ac:dyDescent="0.15">
@@ -4326,7 +4367,7 @@
         <v>127</v>
       </c>
       <c r="B116" s="6" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="E116" s="19" t="s">
         <v>6</v>
@@ -4335,7 +4376,7 @@
         <v>6</v>
       </c>
       <c r="I116" s="32" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="117" spans="1:9" s="27" customFormat="1" ht="30" x14ac:dyDescent="0.15">
@@ -4343,7 +4384,7 @@
         <v>128</v>
       </c>
       <c r="B117" s="27" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="D117" s="26"/>
       <c r="E117" s="26" t="s">
@@ -4355,7 +4396,7 @@
         <v>6</v>
       </c>
       <c r="I117" s="35" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="118" spans="1:9" ht="45" x14ac:dyDescent="0.15">
@@ -4372,7 +4413,7 @@
         <v>6</v>
       </c>
       <c r="I118" s="32" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="119" spans="1:9" ht="15" x14ac:dyDescent="0.15">
@@ -4380,7 +4421,7 @@
         <v>130</v>
       </c>
       <c r="B119" s="6" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="E119" s="19" t="s">
         <v>6</v>
@@ -4389,7 +4430,7 @@
         <v>6</v>
       </c>
       <c r="I119" s="32" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="120" spans="1:9" s="17" customFormat="1" ht="15" x14ac:dyDescent="0.15">
@@ -4397,7 +4438,7 @@
         <v>136</v>
       </c>
       <c r="B120" s="17" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="D120" s="21"/>
       <c r="E120" s="21"/>
@@ -4409,7 +4450,7 @@
         <v>6</v>
       </c>
       <c r="I120" s="33" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="121" spans="1:9" s="27" customFormat="1" ht="60" x14ac:dyDescent="0.15">
@@ -4417,7 +4458,7 @@
         <v>133</v>
       </c>
       <c r="B121" s="27" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D121" s="26" t="s">
         <v>6</v>
@@ -4429,7 +4470,7 @@
         <v>6</v>
       </c>
       <c r="I121" s="35" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
     </row>
     <row r="122" spans="1:9" ht="15" x14ac:dyDescent="0.15">
@@ -4437,16 +4478,16 @@
         <v>135</v>
       </c>
       <c r="B122" s="6" t="s">
+        <v>274</v>
+      </c>
+      <c r="D122" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="H122" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="I122" s="32" t="s">
         <v>275</v>
-      </c>
-      <c r="D122" s="19" t="s">
-        <v>6</v>
-      </c>
-      <c r="H122" s="19" t="s">
-        <v>6</v>
-      </c>
-      <c r="I122" s="32" t="s">
-        <v>276</v>
       </c>
     </row>
     <row r="123" spans="1:9" ht="30" x14ac:dyDescent="0.15">
@@ -4454,7 +4495,7 @@
         <v>131</v>
       </c>
       <c r="B123" s="6" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="E123" s="19" t="s">
         <v>6</v>
@@ -4463,7 +4504,7 @@
         <v>6</v>
       </c>
       <c r="I123" s="32" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="124" spans="1:9" ht="60" x14ac:dyDescent="0.15">
@@ -4471,16 +4512,16 @@
         <v>137</v>
       </c>
       <c r="B124" s="6" t="s">
+        <v>277</v>
+      </c>
+      <c r="D124" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="H124" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="I124" s="32" t="s">
         <v>278</v>
-      </c>
-      <c r="D124" s="19" t="s">
-        <v>6</v>
-      </c>
-      <c r="H124" s="19" t="s">
-        <v>6</v>
-      </c>
-      <c r="I124" s="32" t="s">
-        <v>279</v>
       </c>
     </row>
     <row r="125" spans="1:9" s="27" customFormat="1" ht="15" x14ac:dyDescent="0.15">
@@ -4488,7 +4529,7 @@
         <v>138</v>
       </c>
       <c r="B125" s="27" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="D125" s="26" t="s">
         <v>6</v>
@@ -4500,7 +4541,7 @@
         <v>6</v>
       </c>
       <c r="I125" s="35" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="126" spans="1:9" ht="15" x14ac:dyDescent="0.15">
@@ -4517,7 +4558,7 @@
         <v>6</v>
       </c>
       <c r="I126" s="32" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="127" spans="1:9" ht="15" x14ac:dyDescent="0.15">
@@ -4525,16 +4566,16 @@
         <v>142</v>
       </c>
       <c r="B127" s="6" t="s">
+        <v>281</v>
+      </c>
+      <c r="E127" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="H127" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="I127" s="32" t="s">
         <v>282</v>
-      </c>
-      <c r="E127" s="19" t="s">
-        <v>6</v>
-      </c>
-      <c r="H127" s="19" t="s">
-        <v>6</v>
-      </c>
-      <c r="I127" s="32" t="s">
-        <v>283</v>
       </c>
     </row>
     <row r="128" spans="1:9" s="27" customFormat="1" ht="45" x14ac:dyDescent="0.15">
@@ -4542,7 +4583,7 @@
         <v>141</v>
       </c>
       <c r="B128" s="27" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="D128" s="26" t="s">
         <v>6</v>
@@ -4554,7 +4595,7 @@
         <v>6</v>
       </c>
       <c r="I128" s="35" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="129" spans="1:9" ht="15" x14ac:dyDescent="0.15">
@@ -4571,7 +4612,7 @@
         <v>6</v>
       </c>
       <c r="I129" s="32" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="130" spans="1:9" ht="15" x14ac:dyDescent="0.15">
@@ -4579,7 +4620,7 @@
         <v>144</v>
       </c>
       <c r="B130" s="6" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="E130" s="19" t="s">
         <v>6</v>
@@ -4588,7 +4629,7 @@
         <v>6</v>
       </c>
       <c r="I130" s="32" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="131" spans="1:9" ht="15" x14ac:dyDescent="0.15">
@@ -4605,7 +4646,7 @@
         <v>6</v>
       </c>
       <c r="I131" s="32" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="132" spans="1:9" ht="15" x14ac:dyDescent="0.15">
@@ -4622,7 +4663,7 @@
         <v>6</v>
       </c>
       <c r="I132" s="32" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="133" spans="1:9" ht="15" x14ac:dyDescent="0.15">
@@ -4639,7 +4680,7 @@
         <v>6</v>
       </c>
       <c r="I133" s="32" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="134" spans="1:9" ht="15" x14ac:dyDescent="0.15">
@@ -4647,7 +4688,7 @@
         <v>146</v>
       </c>
       <c r="B134" s="6" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="D134" s="19" t="s">
         <v>6</v>
@@ -4656,7 +4697,7 @@
         <v>6</v>
       </c>
       <c r="I134" s="32" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="135" spans="1:9" ht="135" x14ac:dyDescent="0.15">
@@ -4673,7 +4714,7 @@
         <v>6</v>
       </c>
       <c r="I135" s="32" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="136" spans="1:9" ht="45" x14ac:dyDescent="0.15">
@@ -4681,19 +4722,19 @@
         <v>148</v>
       </c>
       <c r="B136" s="6" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C136" s="32" t="s">
+        <v>288</v>
+      </c>
+      <c r="D136" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="H136" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="I136" s="32" t="s">
         <v>289</v>
-      </c>
-      <c r="D136" s="19" t="s">
-        <v>6</v>
-      </c>
-      <c r="H136" s="19" t="s">
-        <v>6</v>
-      </c>
-      <c r="I136" s="32" t="s">
-        <v>290</v>
       </c>
     </row>
     <row r="137" spans="1:9" ht="30" x14ac:dyDescent="0.15">
@@ -4701,7 +4742,7 @@
         <v>149</v>
       </c>
       <c r="B137" s="6" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="E137" s="19" t="s">
         <v>6</v>
@@ -4710,7 +4751,7 @@
         <v>6</v>
       </c>
       <c r="I137" s="32" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="138" spans="1:9" ht="75" x14ac:dyDescent="0.15">
@@ -4727,7 +4768,7 @@
         <v>6</v>
       </c>
       <c r="I138" s="32" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="139" spans="1:9" ht="15" x14ac:dyDescent="0.15">
@@ -4744,7 +4785,7 @@
         <v>6</v>
       </c>
       <c r="I139" s="32" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="140" spans="1:9" s="17" customFormat="1" ht="30" x14ac:dyDescent="0.15">
@@ -4752,7 +4793,7 @@
         <v>154</v>
       </c>
       <c r="B140" s="17" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="D140" s="21"/>
       <c r="E140" s="21"/>
@@ -4764,7 +4805,7 @@
         <v>6</v>
       </c>
       <c r="I140" s="33" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="141" spans="1:9" s="17" customFormat="1" ht="15" x14ac:dyDescent="0.15">
@@ -4772,7 +4813,7 @@
         <v>153</v>
       </c>
       <c r="B141" s="17" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="D141" s="21"/>
       <c r="E141" s="21"/>
@@ -4784,7 +4825,7 @@
         <v>6</v>
       </c>
       <c r="I141" s="33" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="142" spans="1:9" s="17" customFormat="1" ht="30" x14ac:dyDescent="0.15">
@@ -4792,7 +4833,7 @@
         <v>155</v>
       </c>
       <c r="B142" s="17" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="D142" s="21"/>
       <c r="E142" s="21"/>
@@ -4804,7 +4845,7 @@
         <v>6</v>
       </c>
       <c r="I142" s="33" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="143" spans="1:9" ht="15" x14ac:dyDescent="0.15">
@@ -4812,7 +4853,7 @@
         <v>152</v>
       </c>
       <c r="B143" s="6" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="D143" s="19" t="s">
         <v>6</v>
@@ -4821,7 +4862,7 @@
         <v>6</v>
       </c>
       <c r="I143" s="32" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="144" spans="1:9" s="27" customFormat="1" ht="60" x14ac:dyDescent="0.15">
@@ -4829,7 +4870,7 @@
         <v>156</v>
       </c>
       <c r="B144" s="27" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="D144" s="26" t="s">
         <v>6</v>
@@ -4841,7 +4882,7 @@
         <v>6</v>
       </c>
       <c r="I144" s="35" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="145" spans="1:9" ht="30" x14ac:dyDescent="0.15">
@@ -4858,7 +4899,7 @@
         <v>6</v>
       </c>
       <c r="I145" s="32" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="146" spans="1:9" s="27" customFormat="1" ht="15" x14ac:dyDescent="0.15">
@@ -4866,7 +4907,7 @@
         <v>158</v>
       </c>
       <c r="B146" s="27" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D146" s="26" t="s">
         <v>6</v>
@@ -4878,7 +4919,7 @@
         <v>6</v>
       </c>
       <c r="I146" s="35" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="147" spans="1:9" ht="15" x14ac:dyDescent="0.15">
@@ -4895,7 +4936,7 @@
         <v>6</v>
       </c>
       <c r="I147" s="32" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="148" spans="1:9" ht="45" x14ac:dyDescent="0.15">
@@ -4903,7 +4944,7 @@
         <v>167</v>
       </c>
       <c r="B148" s="6" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="E148" s="19" t="s">
         <v>6</v>
@@ -4912,7 +4953,7 @@
         <v>6</v>
       </c>
       <c r="I148" s="32" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="149" spans="1:9" s="27" customFormat="1" ht="30" x14ac:dyDescent="0.15">
@@ -4920,7 +4961,7 @@
         <v>165</v>
       </c>
       <c r="B149" s="27" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="D149" s="26"/>
       <c r="E149" s="26" t="s">
@@ -4932,7 +4973,7 @@
         <v>6</v>
       </c>
       <c r="I149" s="35" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="150" spans="1:9" ht="15" x14ac:dyDescent="0.15">
@@ -4949,7 +4990,7 @@
         <v>6</v>
       </c>
       <c r="I150" s="32" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="151" spans="1:9" ht="15" x14ac:dyDescent="0.15">
@@ -4966,7 +5007,7 @@
         <v>6</v>
       </c>
       <c r="I151" s="32" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="152" spans="1:9" ht="30" x14ac:dyDescent="0.15">
@@ -4983,7 +5024,7 @@
         <v>6</v>
       </c>
       <c r="I152" s="32" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="153" spans="1:9" ht="15" x14ac:dyDescent="0.15">
@@ -5000,7 +5041,7 @@
         <v>6</v>
       </c>
       <c r="I153" s="32" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="154" spans="1:9" ht="45" x14ac:dyDescent="0.15">
@@ -5017,7 +5058,7 @@
         <v>6</v>
       </c>
       <c r="I154" s="32" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="155" spans="1:9" ht="15" x14ac:dyDescent="0.15">
@@ -5025,16 +5066,16 @@
         <v>189</v>
       </c>
       <c r="B155" s="6" t="s">
+        <v>306</v>
+      </c>
+      <c r="D155" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="H155" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="I155" s="32" t="s">
         <v>307</v>
-      </c>
-      <c r="D155" s="19" t="s">
-        <v>6</v>
-      </c>
-      <c r="H155" s="19" t="s">
-        <v>6</v>
-      </c>
-      <c r="I155" s="32" t="s">
-        <v>308</v>
       </c>
     </row>
     <row r="156" spans="1:9" s="17" customFormat="1" ht="60" x14ac:dyDescent="0.15">
@@ -5042,7 +5083,7 @@
         <v>193</v>
       </c>
       <c r="B156" s="17" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="C156" s="17" t="s">
         <v>35</v>
@@ -5057,7 +5098,7 @@
         <v>6</v>
       </c>
       <c r="I156" s="33" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="157" spans="1:9" ht="15" x14ac:dyDescent="0.15">
@@ -5074,7 +5115,7 @@
         <v>6</v>
       </c>
       <c r="I157" s="32" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="158" spans="1:9" s="27" customFormat="1" ht="30" x14ac:dyDescent="0.15">
@@ -5082,7 +5123,7 @@
         <v>187</v>
       </c>
       <c r="B158" s="27" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="D158" s="26"/>
       <c r="E158" s="26" t="s">
@@ -5094,7 +5135,7 @@
         <v>6</v>
       </c>
       <c r="I158" s="35" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="159" spans="1:9" ht="45" x14ac:dyDescent="0.15">
@@ -5102,7 +5143,7 @@
         <v>186</v>
       </c>
       <c r="B159" s="6" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="D159" s="19" t="s">
         <v>6</v>
@@ -5111,7 +5152,7 @@
         <v>6</v>
       </c>
       <c r="I159" s="32" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="160" spans="1:9" ht="15" x14ac:dyDescent="0.15">
@@ -5119,7 +5160,7 @@
         <v>185</v>
       </c>
       <c r="B160" s="6" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="D160" s="19" t="s">
         <v>6</v>
@@ -5128,7 +5169,7 @@
         <v>6</v>
       </c>
       <c r="I160" s="32" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="161" spans="1:9" ht="15" x14ac:dyDescent="0.15">
@@ -5145,7 +5186,7 @@
         <v>6</v>
       </c>
       <c r="I161" s="32" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="162" spans="1:9" s="27" customFormat="1" ht="30" x14ac:dyDescent="0.15">
@@ -5153,7 +5194,7 @@
         <v>182</v>
       </c>
       <c r="B162" s="27" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="C162" s="35"/>
       <c r="D162" s="26"/>
@@ -5166,7 +5207,7 @@
         <v>6</v>
       </c>
       <c r="I162" s="35" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="163" spans="1:9" ht="15" x14ac:dyDescent="0.15">
@@ -5180,7 +5221,7 @@
         <v>6</v>
       </c>
       <c r="I163" s="32" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="164" spans="1:9" ht="30" x14ac:dyDescent="0.15">
@@ -5194,7 +5235,7 @@
         <v>6</v>
       </c>
       <c r="I164" s="32" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="165" spans="1:9" ht="30" x14ac:dyDescent="0.15">
@@ -5202,13 +5243,13 @@
         <v>179</v>
       </c>
       <c r="B165" s="6" t="s">
+        <v>316</v>
+      </c>
+      <c r="E165" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="I165" s="32" t="s">
         <v>317</v>
-      </c>
-      <c r="E165" s="19" t="s">
-        <v>6</v>
-      </c>
-      <c r="I165" s="32" t="s">
-        <v>318</v>
       </c>
     </row>
     <row r="166" spans="1:9" ht="15" x14ac:dyDescent="0.15">
@@ -5222,7 +5263,7 @@
         <v>6</v>
       </c>
       <c r="I166" s="32" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="167" spans="1:9" s="27" customFormat="1" ht="30" x14ac:dyDescent="0.15">
@@ -5240,7 +5281,7 @@
       <c r="G167" s="47"/>
       <c r="H167" s="26"/>
       <c r="I167" s="35" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="168" spans="1:9" ht="30" x14ac:dyDescent="0.15">
@@ -5254,7 +5295,7 @@
         <v>6</v>
       </c>
       <c r="I168" s="32" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="169" spans="1:9" ht="15" x14ac:dyDescent="0.15">
@@ -5262,13 +5303,13 @@
         <v>174</v>
       </c>
       <c r="B169" s="6" t="s">
+        <v>321</v>
+      </c>
+      <c r="D169" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="I169" s="32" t="s">
         <v>322</v>
-      </c>
-      <c r="D169" s="19" t="s">
-        <v>6</v>
-      </c>
-      <c r="I169" s="32" t="s">
-        <v>323</v>
       </c>
     </row>
     <row r="170" spans="1:9" ht="15" x14ac:dyDescent="0.15">
@@ -5276,13 +5317,13 @@
         <v>173</v>
       </c>
       <c r="B170" s="6" t="s">
+        <v>323</v>
+      </c>
+      <c r="E170" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="I170" s="32" t="s">
         <v>324</v>
-      </c>
-      <c r="E170" s="19" t="s">
-        <v>6</v>
-      </c>
-      <c r="I170" s="32" t="s">
-        <v>325</v>
       </c>
     </row>
     <row r="171" spans="1:9" ht="30" x14ac:dyDescent="0.15">
@@ -5296,15 +5337,15 @@
         <v>6</v>
       </c>
       <c r="I171" s="32" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="172" spans="1:9" s="17" customFormat="1" ht="30" x14ac:dyDescent="0.15">
       <c r="A172" s="17" t="s">
+        <v>326</v>
+      </c>
+      <c r="B172" s="17" t="s">
         <v>327</v>
-      </c>
-      <c r="B172" s="17" t="s">
-        <v>328</v>
       </c>
       <c r="D172" s="21"/>
       <c r="E172" s="21"/>
@@ -5314,12 +5355,12 @@
       <c r="G172" s="48"/>
       <c r="H172" s="21"/>
       <c r="I172" s="33" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="173" spans="1:9" ht="15" x14ac:dyDescent="0.15">
       <c r="A173" s="6" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B173" s="6" t="s">
         <v>168</v>
@@ -5328,18 +5369,18 @@
         <v>6</v>
       </c>
       <c r="I173" s="32" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="174" spans="1:9" s="17" customFormat="1" ht="60" x14ac:dyDescent="0.15">
       <c r="A174" s="17" t="s">
+        <v>331</v>
+      </c>
+      <c r="B174" s="17" t="s">
         <v>332</v>
       </c>
-      <c r="B174" s="17" t="s">
-        <v>333</v>
-      </c>
       <c r="C174" s="17" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="D174" s="21"/>
       <c r="E174" s="21"/>
@@ -5349,12 +5390,12 @@
       <c r="G174" s="48"/>
       <c r="H174" s="21"/>
       <c r="I174" s="33" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="175" spans="1:9" ht="15" x14ac:dyDescent="0.15">
       <c r="A175" s="6" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="B175" s="6" t="s">
         <v>74</v>
@@ -5363,12 +5404,12 @@
         <v>6</v>
       </c>
       <c r="I175" s="32" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="176" spans="1:9" ht="15" x14ac:dyDescent="0.15">
       <c r="A176" s="6" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="B176" s="6" t="s">
         <v>116</v>
@@ -5377,12 +5418,12 @@
         <v>6</v>
       </c>
       <c r="I176" s="32" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="177" spans="1:9" s="27" customFormat="1" ht="15" x14ac:dyDescent="0.15">
       <c r="A177" s="27" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="B177" s="27" t="s">
         <v>28</v>
@@ -5395,15 +5436,15 @@
       <c r="G177" s="47"/>
       <c r="H177" s="26"/>
       <c r="I177" s="35" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="178" spans="1:9" s="17" customFormat="1" ht="30" x14ac:dyDescent="0.15">
       <c r="A178" s="17" t="s">
+        <v>340</v>
+      </c>
+      <c r="B178" s="17" t="s">
         <v>341</v>
-      </c>
-      <c r="B178" s="17" t="s">
-        <v>342</v>
       </c>
       <c r="D178" s="21"/>
       <c r="E178" s="21" t="s">
@@ -5413,26 +5454,26 @@
       <c r="G178" s="48"/>
       <c r="H178" s="21"/>
       <c r="I178" s="33" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="179" spans="1:9" ht="30" x14ac:dyDescent="0.15">
       <c r="A179" s="6" t="s">
+        <v>343</v>
+      </c>
+      <c r="B179" s="6" t="s">
         <v>344</v>
       </c>
-      <c r="B179" s="6" t="s">
+      <c r="E179" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="I179" s="32" t="s">
         <v>345</v>
-      </c>
-      <c r="E179" s="19" t="s">
-        <v>6</v>
-      </c>
-      <c r="I179" s="32" t="s">
-        <v>346</v>
       </c>
     </row>
     <row r="180" spans="1:9" s="27" customFormat="1" ht="60" x14ac:dyDescent="0.15">
       <c r="A180" s="27" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B180" s="27" t="s">
         <v>15</v>
@@ -5445,15 +5486,15 @@
       <c r="G180" s="47"/>
       <c r="H180" s="26"/>
       <c r="I180" s="35" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
     </row>
     <row r="181" spans="1:9" s="17" customFormat="1" ht="45" x14ac:dyDescent="0.15">
       <c r="A181" s="17" t="s">
+        <v>348</v>
+      </c>
+      <c r="B181" s="17" t="s">
         <v>349</v>
-      </c>
-      <c r="B181" s="17" t="s">
-        <v>350</v>
       </c>
       <c r="D181" s="21"/>
       <c r="E181" s="21"/>
@@ -5463,12 +5504,12 @@
       <c r="G181" s="48"/>
       <c r="H181" s="21"/>
       <c r="I181" s="33" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="182" spans="1:9" ht="30" x14ac:dyDescent="0.15">
       <c r="A182" s="6" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="B182" s="6" t="s">
         <v>15</v>
@@ -5477,26 +5518,26 @@
         <v>6</v>
       </c>
       <c r="I182" s="32" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
     </row>
     <row r="183" spans="1:9" ht="15" x14ac:dyDescent="0.15">
       <c r="A183" s="6" t="s">
+        <v>353</v>
+      </c>
+      <c r="B183" s="6" t="s">
         <v>354</v>
       </c>
-      <c r="B183" s="6" t="s">
+      <c r="E183" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="I183" s="32" t="s">
         <v>355</v>
-      </c>
-      <c r="E183" s="19" t="s">
-        <v>6</v>
-      </c>
-      <c r="I183" s="32" t="s">
-        <v>356</v>
       </c>
     </row>
     <row r="184" spans="1:9" ht="15" x14ac:dyDescent="0.15">
       <c r="A184" s="6" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B184" s="6" t="s">
         <v>76</v>
@@ -5505,21 +5546,21 @@
         <v>6</v>
       </c>
       <c r="I184" s="32" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="185" spans="1:9" ht="90" x14ac:dyDescent="0.15">
       <c r="A185" s="6" t="s">
+        <v>358</v>
+      </c>
+      <c r="B185" s="6" t="s">
         <v>359</v>
       </c>
-      <c r="B185" s="6" t="s">
+      <c r="F185" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="I185" s="32" t="s">
         <v>360</v>
-      </c>
-      <c r="F185" s="19" t="s">
-        <v>6</v>
-      </c>
-      <c r="I185" s="32" t="s">
-        <v>361</v>
       </c>
     </row>
   </sheetData>

</xml_diff>